<commit_message>
commiting the latest TestData
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a212613162/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2E71B91A-A7AD-7A43-9E65-F42A278E9061}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{86502604-A505-CF4D-B6BC-3FD830298713}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>Scenario7OPDOC</t>
+  </si>
+  <si>
+    <t>ExploreChildSearch</t>
+  </si>
+  <si>
+    <t>IssueText</t>
+  </si>
+  <si>
+    <t>BillingType</t>
+  </si>
+  <si>
+    <t>AUTOMATION SEARCH</t>
+  </si>
+  <si>
+    <t>scenario5</t>
+  </si>
+  <si>
+    <t>Work Orders</t>
+  </si>
+  <si>
+    <t>Billing Type cannot be Loan</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>DATA_SANITY5</t>
+  </si>
+  <si>
+    <t>SANITY5</t>
+  </si>
+  <si>
+    <t>SANITY6</t>
+  </si>
+  <si>
+    <t>DATA_SANITY6</t>
+  </si>
+  <si>
+    <t>Cases</t>
   </si>
 </sst>
 </file>
@@ -565,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -577,7 +616,7 @@
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="8" width="9.83203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -780,7 +819,7 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -795,6 +834,92 @@
       <c r="E7" s="11" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="8" spans="1:20" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:20" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
committing scenario 7-API updates and navigatetoWO functions
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a212613162/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{86502604-A505-CF4D-B6BC-3FD830298713}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6ABDB66-8436-8F4A-B1AB-76565B7B9F34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -607,7 +607,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -797,12 +797,14 @@
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="9"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -829,9 +831,12 @@
         <v>31</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commiting changes to scenario2,7 and testdata file
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6ABDB66-8436-8F4A-B1AB-76565B7B9F34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0F106733-491E-8340-A505-85E46D1B77B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -607,13 +607,13 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -750,9 +750,11 @@
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -773,15 +775,17 @@
         <v>29</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="7"/>
       <c r="G5" s="7"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -825,7 +829,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
pushing the merged Excel Data Sheet
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512D611-1F43-6B45-8C41-2475F9D9A6B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -201,12 +202,36 @@
   </si>
   <si>
     <t>RS-10554-mapping-manual</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>EditProcessName</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>Manual_Checklist_Edit_WO_PROCESS</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_2_RS-10578_DVR</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_2_RS-10578_DVR</t>
+  </si>
+  <si>
+    <t>Manual_SCN_Checklist_2_RS-10578_ DVR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,11 +666,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1074,6 +1099,94 @@
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
     </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pushing the testData File with checklist scenario
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512D611-1F43-6B45-8C41-2475F9D9A6B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7D3885-9CC2-3E47-9863-66C2B1F67010}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Manual_SCN_Checklist_2_RS-10578_ DVR</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>Manual_SCN_Checklist_3_RS-10579_ Entry_Exit_Criteria</t>
   </si>
 </sst>
 </file>
@@ -667,19 +676,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="8" width="9.83203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -1187,6 +1196,46 @@
       </c>
       <c r="G17" s="5"/>
     </row>
+    <row r="18" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pushing latest TestData File.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7D3885-9CC2-3E47-9863-66C2B1F67010}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B265C-8E09-FE4B-B2B9-2FFDB7472819}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -234,7 +234,16 @@
     <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
   </si>
   <si>
-    <t>Manual_SCN_Checklist_3_RS-10579_ Entry_Exit_Criteria</t>
+    <t>ManualSCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_4_RS10580_Checklist_Sections</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_4_RS-10580_Sections</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
   </si>
 </sst>
 </file>
@@ -676,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1236,6 +1245,46 @@
         <v>62</v>
       </c>
     </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pushing the latest TestDataFile with RS10544_SOU
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B020E5-25B3-9444-82E5-0B27A29B8FBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -264,12 +265,21 @@
   </si>
   <si>
     <t>RS_10554_7920189427</t>
+  </si>
+  <si>
+    <t>SCN_SourceObjectUpdate_RS_10544</t>
+  </si>
+  <si>
+    <t>Data_SCN_SourceObjectUpdate_RS_10544</t>
+  </si>
+  <si>
+    <t>Manual_RS_10544_SOU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -720,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1447,6 +1457,40 @@
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
     </row>
+    <row r="26" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pushing in 10544 along with few changes
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B020E5-25B3-9444-82E5-0B27A29B8FBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDA7B09-B392-1D41-AC2D-4A600F739F89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
pushing in the TESTDATA file after merger missed ones.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15DEB3A-AB44-D942-9898-E65CCE5B9EBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -245,12 +246,27 @@
     <t>RS-10557_mapping</t>
   </si>
   <si>
+    <t>RS_10557_592018205141</t>
+  </si>
+  <si>
     <t>RS-10556_mapping</t>
   </si>
   <si>
+    <t>Work Order</t>
+  </si>
+  <si>
+    <t>RS_10556_mapping</t>
+  </si>
+  <si>
     <t>WorkOrder Number</t>
   </si>
   <si>
+    <t>WO-00002089</t>
+  </si>
+  <si>
+    <t>RS_10554_7920189427</t>
+  </si>
+  <si>
     <t>SCN_SourceObjectUpdate_RS_10544</t>
   </si>
   <si>
@@ -260,13 +276,13 @@
     <t>Manual_RS_10544_SOU</t>
   </si>
   <si>
-    <t>RS_10554_field_mapping</t>
-  </si>
-  <si>
-    <t>RS_10556_149201814101</t>
-  </si>
-  <si>
-    <t>WO-00002321</t>
+    <t>SCN_DVR_RS_10550</t>
+  </si>
+  <si>
+    <t>Data_SCN_DVR_RS_10550</t>
+  </si>
+  <si>
+    <t>Manual_SCN_10550_DVR</t>
   </si>
   <si>
     <t>RS_10566_Acc_Pro_History</t>
@@ -276,16 +292,13 @@
   </si>
   <si>
     <t>View Work Order</t>
-  </si>
-  <si>
-    <t>RS_10557_Child_Mapping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,12 +335,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF424242"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +379,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -383,10 +410,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -411,9 +439,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -725,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -737,11 +768,10 @@
     <col min="1" max="1" width="39.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="8" width="9.83203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="13" max="13" width="14.83203125" customWidth="1"/>
   </cols>
@@ -1139,7 +1169,7 @@
         <v>56</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="11"/>
@@ -1367,8 +1397,8 @@
       <c r="C23" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>83</v>
+      <c r="D23" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -1390,7 +1420,7 @@
     </row>
     <row r="24" spans="1:21" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>19</v>
@@ -1402,7 +1432,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1422,19 +1452,19 @@
     </row>
     <row r="25" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -1455,7 +1485,7 @@
     </row>
     <row r="26" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>19</v>
@@ -1472,13 +1502,13 @@
     </row>
     <row r="27" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>43</v>
@@ -1487,70 +1517,73 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-    </row>
-    <row r="29" spans="1:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="17" t="s">
+    </row>
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
committing final changes necessary to run with sahi.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15DEB3A-AB44-D942-9898-E65CCE5B9EBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB7E1EC-A3E9-EE42-B8FA-B59C0EE39D33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Data_SCN_DVR_RS_10550</t>
   </si>
   <si>
-    <t>Manual_SCN_10550_DVR</t>
-  </si>
-  <si>
     <t>RS_10566_Acc_Pro_History</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>View Work Order</t>
+  </si>
+  <si>
+    <t>AUTO_RS10550_DVR</t>
   </si>
 </sst>
 </file>
@@ -339,6 +339,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -759,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1530,9 +1531,7 @@
       <c r="D28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
@@ -1542,18 +1541,16 @@
         <v>41</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>19</v>
@@ -1562,7 +1559,7 @@
         <v>38</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>58</v>
@@ -1570,7 +1567,7 @@
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>41</v>
@@ -1579,10 +1576,10 @@
         <v>43</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes of RS-10539
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20919"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="105">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>IB1053820920189437</t>
+  </si>
+  <si>
+    <t>SCN_GetPriceSCON_RS_10539</t>
+  </si>
+  <si>
+    <t>Product1 Name </t>
+  </si>
+  <si>
+    <t>Product2 Name</t>
+  </si>
+  <si>
+    <t>ServiceContract Name</t>
   </si>
 </sst>
 </file>
@@ -791,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -1692,6 +1704,23 @@
         <v>100</v>
       </c>
     </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pushing RS-10532 for the test case
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20919"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -321,16 +321,16 @@
     <t>Installed Product Name</t>
   </si>
   <si>
-    <t>WO-00002485</t>
-  </si>
-  <si>
-    <t>P1053820920189436</t>
+    <t>WO-00002616</t>
+  </si>
+  <si>
+    <t>P105382592018152038</t>
   </si>
   <si>
     <t>AutoA10538_Auto</t>
   </si>
   <si>
-    <t>IB1053820920189437</t>
+    <t>IB105382592018152039</t>
   </si>
   <si>
     <t>SCN_GetPriceSCON_RS_10539</t>
@@ -355,22 +355,12 @@
   </si>
   <si>
     <t>AutoScon259201812555</t>
-  </si>
-  <si>
-    <t>WO-00002616</t>
-  </si>
-  <si>
-    <t>P105382592018152038</t>
-  </si>
-  <si>
-    <t>IB105382592018152039</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -825,23 +815,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1714,16 +1704,16 @@
         <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
         <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
@@ -1755,6 +1745,14 @@
       </c>
       <c r="E37" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushign changes for Test Data
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="110">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>AutoScon259201812555</t>
+  </si>
+  <si>
+    <t>SCN_GetPriceNotCovered_RS_10532</t>
   </si>
 </sst>
 </file>
@@ -815,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -1734,6 +1737,9 @@
       </c>
     </row>
     <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
       <c r="B37" t="s">
         <v>105</v>
       </c>
@@ -1749,10 +1755,15 @@
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1">
+      <c r="A39" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing data file,scripts for 585,587
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682080E3-8C8F-064F-AA5A-06C239F1C818}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A76B0EE-5B75-124B-8B7B-44150251E872}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="124">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -360,30 +360,53 @@
     <t>SCN_GetPriceNotCovered_RS_10532</t>
   </si>
   <si>
-    <t>WO-00002770</t>
-  </si>
-  <si>
-    <t>WO-00002777</t>
-  </si>
-  <si>
-    <t>WO-00002779</t>
-  </si>
-  <si>
-    <t>WO-00002782</t>
-  </si>
-  <si>
-    <t>WO-00002786</t>
-  </si>
-  <si>
     <t>WO-00002804</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_1_RS-10585</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_1_RS-10585</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10585_inProg</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_allversions</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
+  </si>
+  <si>
+    <t>ChecklistName_AllVersions</t>
+  </si>
+  <si>
+    <t>ChecklistName_FirstVersion</t>
+  </si>
+  <si>
+    <t>ChecklistName_LastVersion</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,26 +860,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +935,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -949,7 +973,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -972,7 +996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1003,7 +1027,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1023,7 +1047,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1057,7 +1081,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1">
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1101,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1111,7 +1135,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
@@ -1131,7 +1155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -1169,7 +1193,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>50</v>
       </c>
@@ -1208,7 +1232,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>55</v>
       </c>
@@ -1238,7 +1262,7 @@
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1268,7 +1292,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1291,7 +1315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>60</v>
       </c>
@@ -1314,7 +1338,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1">
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>63</v>
       </c>
@@ -1334,7 +1358,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>64</v>
       </c>
@@ -1354,7 +1378,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>66</v>
       </c>
@@ -1374,7 +1398,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -1394,7 +1418,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -1414,7 +1438,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>70</v>
       </c>
@@ -1434,7 +1458,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>72</v>
       </c>
@@ -1464,7 +1488,7 @@
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1495,7 +1519,7 @@
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
     </row>
-    <row r="24" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="24" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>74</v>
       </c>
@@ -1527,7 +1551,7 @@
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1560,7 +1584,7 @@
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>79</v>
       </c>
@@ -1577,7 +1601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>80</v>
       </c>
@@ -1594,7 +1618,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
@@ -1609,7 +1633,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>83</v>
       </c>
@@ -1624,7 +1648,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1">
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>85</v>
       </c>
@@ -1641,7 +1665,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
@@ -1658,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -1681,7 +1705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1">
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>89</v>
       </c>
@@ -1704,7 +1728,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>92</v>
       </c>
@@ -1721,7 +1745,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1">
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1738,7 +1762,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1">
+    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
@@ -1755,7 +1779,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -1772,7 +1796,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1">
+    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>109</v>
       </c>
@@ -1780,13 +1804,124 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1">
+    <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>109</v>
       </c>
       <c r="B39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>115</v>
       </c>
+      <c r="B43" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" t="s">
+        <v>117</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="F44" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
pushing changes of RS-10534.java
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20919"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_DAB568F4E83DBE4C96D2FA2EB81DF19D7D9DC7B2" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="179020" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="134">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -371,12 +372,27 @@
     <t>ManualSCN_ChecklistOPDOC_3_RS-10585_inProg</t>
   </si>
   <si>
+    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>ChecklistName_AllVersions</t>
+  </si>
+  <si>
+    <t>ChecklistName_FirstVersion</t>
+  </si>
+  <si>
+    <t>ChecklistName_LastVersion</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587_allversions</t>
   </si>
   <si>
-    <t>Data_SCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
   </si>
   <si>
@@ -386,21 +402,6 @@
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
-    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
-  </si>
-  <si>
-    <t>ChecklistName_AllVersions</t>
-  </si>
-  <si>
-    <t>ChecklistName_FirstVersion</t>
-  </si>
-  <si>
-    <t>ChecklistName_LastVersion</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
     <t>RS_10565_Recent_Items</t>
   </si>
   <si>
@@ -426,13 +427,16 @@
   </si>
   <si>
     <t>a240t000000GglLAAS</t>
+  </si>
+  <si>
+    <t>SCN_GetPrice_RS_10534</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -575,8 +579,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -892,28 +894,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +970,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1006,7 +1008,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1029,7 +1031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1060,7 +1062,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1080,7 +1082,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1114,7 +1116,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="15" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>38</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1168,7 +1170,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="15" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -1226,7 +1228,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="15" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>50</v>
       </c>
@@ -1265,7 +1267,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>55</v>
       </c>
@@ -1295,7 +1297,7 @@
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1325,7 +1327,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="15" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>60</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="15" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>63</v>
       </c>
@@ -1391,7 +1393,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="15" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>64</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="15" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>66</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="15" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="15" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="15" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>70</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>72</v>
       </c>
@@ -1521,7 +1523,7 @@
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1552,7 +1554,7 @@
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
     </row>
-    <row r="24" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>74</v>
       </c>
@@ -1584,7 +1586,7 @@
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1617,7 +1619,7 @@
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="15" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>79</v>
       </c>
@@ -1634,7 +1636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="15" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>80</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="15" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
@@ -1666,7 +1668,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="15" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>83</v>
       </c>
@@ -1681,7 +1683,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>85</v>
       </c>
@@ -1698,7 +1700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="15" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" ht="15" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="15" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>89</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="15" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>92</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="15" customHeight="1">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" ht="15" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
@@ -1812,7 +1814,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="15" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>109</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="15" customHeight="1">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" ht="15" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>111</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" ht="15" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>112</v>
       </c>
@@ -1888,12 +1890,12 @@
         <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>15</v>
@@ -1905,13 +1907,13 @@
         <v>30</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>59</v>
@@ -1920,9 +1922,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" ht="15" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>32</v>
@@ -1934,22 +1936,22 @@
         <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G43" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>62</v>
       </c>
       <c r="I43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A44" s="10" t="s">
         <v>124</v>
       </c>
@@ -1981,23 +1983,22 @@
       <c r="S44" s="11"/>
       <c r="T44" s="11"/>
     </row>
-    <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="45" spans="1:21" ht="15" customHeight="1">
+      <c r="A45" t="s">
         <v>124</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" t="s">
         <v>32</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="17"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
@@ -2014,7 +2015,7 @@
       <c r="T45" s="8"/>
       <c r="U45" s="8"/>
     </row>
-    <row r="46" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A46" s="10" t="s">
         <v>129</v>
       </c>
@@ -2048,23 +2049,23 @@
       <c r="S46" s="11"/>
       <c r="T46" s="11"/>
     </row>
-    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+    <row r="47" spans="1:21" ht="15" customHeight="1">
+      <c r="A47" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" t="s">
         <v>127</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" t="s">
         <v>132</v>
       </c>
       <c r="G47" s="8"/>
@@ -2083,6 +2084,19 @@
       <c r="T47" s="8"/>
       <c r="U47" s="8"/>
     </row>
+    <row r="48" spans="1:21" ht="15" customHeight="1">
+      <c r="A48" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15" customHeight="1">
+      <c r="A49" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes of RS-10534 Rs-10539
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="171">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>WO-00003100</t>
+  </si>
+  <si>
+    <t>WO-00003104</t>
+  </si>
+  <si>
+    <t>WO-00003105</t>
   </si>
 </sst>
 </file>
@@ -2527,10 +2533,10 @@
         <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reuploading testdata file with changes as the new commit does not have my excel data
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10A198CB-A686-D14F-B3D9-4399C3D27E58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629D7C60-30D2-2248-9F4A-73F3CB575D9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="149">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
   </si>
   <si>
-    <t>ManualSCN_Checklist_4_RS10580_Checklist_Sections</t>
-  </si>
-  <si>
     <t>RS-10557_mapping</t>
   </si>
   <si>
@@ -354,18 +351,9 @@
     <t>Installed Product Name</t>
   </si>
   <si>
-    <t>WO-00002616</t>
-  </si>
-  <si>
-    <t>P105382592018152038</t>
-  </si>
-  <si>
     <t>AutoA10538_Auto</t>
   </si>
   <si>
-    <t>IB105382592018152039</t>
-  </si>
-  <si>
     <t>SCN_GetPriceSCON_RS_10539</t>
   </si>
   <si>
@@ -378,18 +366,6 @@
     <t>ServiceContract Name</t>
   </si>
   <si>
-    <t>WO-00002602</t>
-  </si>
-  <si>
-    <t>P1053925920181250191</t>
-  </si>
-  <si>
-    <t>P1053925920181250192</t>
-  </si>
-  <si>
-    <t>AutoScon259201810214</t>
-  </si>
-  <si>
     <t>AutoA10539_Auto</t>
   </si>
   <si>
@@ -471,45 +447,6 @@
     <t>Work Order Number2</t>
   </si>
   <si>
-    <t>WO-00003028</t>
-  </si>
-  <si>
-    <t>WO-00003034</t>
-  </si>
-  <si>
-    <t>WO-00003036</t>
-  </si>
-  <si>
-    <t>WO-00003041</t>
-  </si>
-  <si>
-    <t>WO-00003044</t>
-  </si>
-  <si>
-    <t>WO-00003046</t>
-  </si>
-  <si>
-    <t>WO-00003051</t>
-  </si>
-  <si>
-    <t>WO-00003053</t>
-  </si>
-  <si>
-    <t>WO-00003056</t>
-  </si>
-  <si>
-    <t>WO-00003057</t>
-  </si>
-  <si>
-    <t>WO-00003059</t>
-  </si>
-  <si>
-    <t>P10538410201815407</t>
-  </si>
-  <si>
-    <t>IB10538410201815408</t>
-  </si>
-  <si>
     <t>WO-00003063</t>
   </si>
   <si>
@@ -531,24 +468,20 @@
     <t>AutoScon5102018103339</t>
   </si>
   <si>
-    <t>WO-00003099</t>
-  </si>
-  <si>
-    <t>WO-00003100</t>
-  </si>
-  <si>
     <t>WO-00003104</t>
   </si>
   <si>
     <t>WO-00003105</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_4_RS-10580_Checklist_Sections</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1016,25 +949,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1021,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1127,7 +1059,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1082,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1181,7 +1113,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1201,7 +1133,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1235,7 +1167,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1">
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>38</v>
       </c>
@@ -1255,7 +1187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1289,7 +1221,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
@@ -1309,7 +1241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -1347,7 +1279,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>50</v>
       </c>
@@ -1386,7 +1318,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>55</v>
       </c>
@@ -1424,7 +1356,7 @@
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -1463,7 +1395,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>58</v>
       </c>
@@ -1501,7 +1433,7 @@
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>59</v>
       </c>
@@ -1540,7 +1472,7 @@
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
     </row>
-    <row r="16" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>62</v>
       </c>
@@ -1578,7 +1510,7 @@
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>63</v>
       </c>
@@ -1617,7 +1549,7 @@
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
     </row>
-    <row r="18" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1587,7 @@
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>65</v>
       </c>
@@ -1694,7 +1626,7 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
     </row>
-    <row r="20" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
@@ -1724,7 +1656,7 @@
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1754,7 +1686,7 @@
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>69</v>
       </c>
@@ -1777,7 +1709,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>71</v>
       </c>
@@ -1800,7 +1732,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
@@ -1820,7 +1752,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>75</v>
       </c>
@@ -1840,7 +1772,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
@@ -1860,7 +1792,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>78</v>
       </c>
@@ -1880,7 +1812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>80</v>
       </c>
@@ -1900,7 +1832,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>81</v>
       </c>
@@ -1914,15 +1846,15 @@
         <v>34</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>15</v>
@@ -1950,9 +1882,9 @@
       <c r="S30" s="11"/>
       <c r="T30" s="11"/>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>32</v>
@@ -1961,7 +1893,7 @@
         <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -1981,9 +1913,9 @@
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
     </row>
-    <row r="32" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="32" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>15</v>
@@ -1995,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -2013,21 +1945,21 @@
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
     </row>
-    <row r="33" spans="1:21" ht="15" customHeight="1">
+    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" t="s">
         <v>87</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>88</v>
-      </c>
-      <c r="E33" t="s">
-        <v>89</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -2046,9 +1978,9 @@
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
     </row>
-    <row r="34" spans="1:21" ht="15" customHeight="1">
+    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>15</v>
@@ -2063,15 +1995,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1">
+    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>34</v>
@@ -2080,9 +2012,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1">
+    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>15</v>
@@ -2095,24 +2027,24 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:21" ht="15" customHeight="1">
+    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="38" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>15</v>
@@ -2121,15 +2053,15 @@
         <v>30</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1">
+    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>32</v>
@@ -2138,15 +2070,15 @@
         <v>34</v>
       </c>
       <c r="D39" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="15" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>15</v>
@@ -2167,9 +2099,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15" customHeight="1">
+    <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>32</v>
@@ -2181,108 +2113,108 @@
         <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" ht="15" customHeight="1">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="C42" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="D42" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="16" t="s">
+    </row>
+    <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" ht="15" customHeight="1">
-      <c r="A43" t="s">
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B43" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E43" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="15" customHeight="1">
-      <c r="A44" s="3" t="s">
+      <c r="E44" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="16" t="s">
+    </row>
+    <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="B46" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
         <v>114</v>
       </c>
-      <c r="E44" s="16" t="s">
+    </row>
+    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
-      <c r="A45" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" t="s">
-        <v>164</v>
-      </c>
-      <c r="D45" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" t="s">
-        <v>166</v>
-      </c>
-      <c r="F45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="15" customHeight="1">
-      <c r="A46" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="15" customHeight="1">
-      <c r="A47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B47" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="15" customHeight="1">
-      <c r="A48" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>15</v>
@@ -2303,9 +2235,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="15" customHeight="1">
+    <row r="49" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>32</v>
@@ -2317,18 +2249,18 @@
         <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G49" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="15" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>15</v>
@@ -2340,13 +2272,13 @@
         <v>30</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>70</v>
@@ -2355,9 +2287,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15" customHeight="1">
+    <row r="51" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>32</v>
@@ -2369,24 +2301,24 @@
         <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G51" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>73</v>
       </c>
       <c r="I51" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>15</v>
@@ -2395,10 +2327,10 @@
         <v>30</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -2416,9 +2348,9 @@
       <c r="S52" s="11"/>
       <c r="T52" s="11"/>
     </row>
-    <row r="53" spans="1:21" ht="15" customHeight="1">
+    <row r="53" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B53" t="s">
         <v>32</v>
@@ -2427,10 +2359,10 @@
         <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
@@ -2448,9 +2380,9 @@
       <c r="T53" s="8"/>
       <c r="U53" s="8"/>
     </row>
-    <row r="54" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="54" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>15</v>
@@ -2459,13 +2391,13 @@
         <v>30</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -2482,9 +2414,9 @@
       <c r="S54" s="11"/>
       <c r="T54" s="11"/>
     </row>
-    <row r="55" spans="1:21" ht="15" customHeight="1">
+    <row r="55" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
@@ -2493,13 +2425,13 @@
         <v>34</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F55" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -2517,26 +2449,26 @@
       <c r="T55" s="8"/>
       <c r="U55" s="8"/>
     </row>
-    <row r="56" spans="1:21" ht="15" customHeight="1">
+    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" ht="15" customHeight="1">
-      <c r="A57" t="s">
-        <v>145</v>
-      </c>
-      <c r="B57" t="s">
-        <v>169</v>
-      </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes of RS-10536
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="175">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>WO-00003324</t>
+  </si>
+  <si>
+    <t>WO-00003325</t>
   </si>
 </sst>
 </file>
@@ -1485,8 +1488,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="42.28515625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1522,7 +1525,7 @@
         <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes of TestData
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_A591CCD61FB231D02A34A3D4F37152F691A5BD46" xr6:coauthVersionLast="39" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_A591CCD61FB231D02A34A3D4F37152F691A5BD46" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="920" windowWidth="28800" windowHeight="16260" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="920" windowWidth="28800" windowHeight="16260" firstSheet="12" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="175">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -313,6 +313,9 @@
     <t>Account Name</t>
   </si>
   <si>
+    <t>Installed Product Name</t>
+  </si>
+  <si>
     <t>WO-00003261</t>
   </si>
   <si>
@@ -328,15 +331,15 @@
     <t>Auto_1053912102018133339</t>
   </si>
   <si>
+    <t>IB1053915102018144235</t>
+  </si>
+  <si>
     <t>SCN_GetPrice_RS_10538</t>
   </si>
   <si>
     <t xml:space="preserve">Product Name </t>
   </si>
   <si>
-    <t>Installed Product Name</t>
-  </si>
-  <si>
     <t>WO-00003256</t>
   </si>
   <si>
@@ -352,6 +355,9 @@
     <t>SCN_GetPrice_RS_10536</t>
   </si>
   <si>
+    <t>WO-00003370</t>
+  </si>
+  <si>
     <t>SCN_ChecklistOPDOC_2_RS-10586</t>
   </si>
   <si>
@@ -584,22 +590,12 @@
   </si>
   <si>
     <t>SFM_Auto_2372018162541</t>
-  </si>
-  <si>
-    <t>WO-00003324</t>
-  </si>
-  <si>
-    <t>WO-00003325</t>
-  </si>
-  <si>
-    <t>WO-00003370</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -764,10 +760,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1089,15 +1085,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1269,11 +1265,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="51.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1349,25 +1349,31 @@
       <c r="F2" s="16" t="s">
         <v>81</v>
       </c>
+      <c r="G2" s="16" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1385,8 +1391,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1446,36 +1452,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>81</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1487,12 +1493,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94480E05-B7FA-4DD5-89EE-C6E7F7328DF1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{62312496-B7DB-5A1E-BE5B-04E292D686FF}"/>
+    <sheetView workbookViewId="0" xr3:uid="{62312496-B7DB-5A1E-BE5B-04E292D686FF}"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1514,7 +1520,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1525,10 +1531,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1609,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1626,7 +1632,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -1638,13 +1644,13 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1719,7 +1725,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -1728,7 +1734,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>61</v>
@@ -1736,7 +1742,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -1745,10 +1751,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1829,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1838,13 +1844,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
@@ -1866,7 +1872,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1926,7 +1932,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1943,13 +1949,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
@@ -2030,7 +2036,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2062,19 +2068,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2165,7 +2171,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2195,16 +2201,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2331,7 +2337,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2391,7 +2397,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -2411,7 +2417,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -2423,7 +2429,7 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
@@ -2444,7 +2450,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2504,7 +2510,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -2524,7 +2530,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -2536,7 +2542,7 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
@@ -2614,7 +2620,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -2634,7 +2640,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -2646,7 +2652,7 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
@@ -2724,7 +2730,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -2747,7 +2753,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -2759,10 +2765,10 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>68</v>
@@ -2840,7 +2846,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2870,16 +2876,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2970,7 +2976,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2982,16 +2988,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3008,28 +3014,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3117,7 +3123,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3129,16 +3135,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3155,28 +3161,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3264,7 +3270,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3276,16 +3282,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3302,28 +3308,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3411,7 +3417,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3423,16 +3429,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3449,7 +3455,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -3458,19 +3464,19 @@
         <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3558,7 +3564,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3570,16 +3576,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3596,28 +3602,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3787,7 +3793,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3847,7 +3853,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -3859,10 +3865,10 @@
         <v>23</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -3881,22 +3887,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3971,7 +3977,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -4005,7 +4011,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -4017,10 +4023,10 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4038,7 +4044,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4098,7 +4104,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -4107,19 +4113,19 @@
         <v>57</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4136,30 +4142,30 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>22</v>
@@ -4190,7 +4196,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>27</v>
@@ -4202,7 +4208,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="6"/>

</xml_diff>

<commit_message>
pushing changes of RS_10531
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_A591CCD61FB231D02A34A3D4F37152F691A5BD46" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="920" windowWidth="28800" windowHeight="16260" firstSheet="12" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="920" windowWidth="28800" windowHeight="16260" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -24,28 +24,29 @@
     <sheet name="RS_10585" sheetId="26" r:id="rId9"/>
     <sheet name="RS_10532" sheetId="25" r:id="rId10"/>
     <sheet name="RS_10539" sheetId="24" r:id="rId11"/>
-    <sheet name="RS_10538" sheetId="23" r:id="rId12"/>
-    <sheet name="RS_10536" sheetId="34" r:id="rId13"/>
-    <sheet name="RS_10586" sheetId="22" r:id="rId14"/>
-    <sheet name="RS_10566" sheetId="21" r:id="rId15"/>
-    <sheet name="RS_10550" sheetId="20" r:id="rId16"/>
-    <sheet name="RS_10544" sheetId="19" r:id="rId17"/>
-    <sheet name="RS_10556" sheetId="18" r:id="rId18"/>
-    <sheet name="RS_10557" sheetId="17" r:id="rId19"/>
-    <sheet name="RS_10580" sheetId="16" r:id="rId20"/>
-    <sheet name="RS_10579" sheetId="14" r:id="rId21"/>
-    <sheet name="RS_10578" sheetId="13" r:id="rId22"/>
-    <sheet name="RS_10577" sheetId="12" r:id="rId23"/>
-    <sheet name="RS_10554" sheetId="11" r:id="rId24"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId25"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId26"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId27"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId28"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId29"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId30"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId31"/>
-    <sheet name="RS_2389" sheetId="2" r:id="rId32"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId33"/>
+    <sheet name="RS_10531" sheetId="35" r:id="rId12"/>
+    <sheet name="RS_10538" sheetId="23" r:id="rId13"/>
+    <sheet name="RS_10536" sheetId="34" r:id="rId14"/>
+    <sheet name="RS_10586" sheetId="22" r:id="rId15"/>
+    <sheet name="RS_10566" sheetId="21" r:id="rId16"/>
+    <sheet name="RS_10550" sheetId="20" r:id="rId17"/>
+    <sheet name="RS_10544" sheetId="19" r:id="rId18"/>
+    <sheet name="RS_10556" sheetId="18" r:id="rId19"/>
+    <sheet name="RS_10557" sheetId="17" r:id="rId20"/>
+    <sheet name="RS_10580" sheetId="16" r:id="rId21"/>
+    <sheet name="RS_10579" sheetId="14" r:id="rId22"/>
+    <sheet name="RS_10578" sheetId="13" r:id="rId23"/>
+    <sheet name="RS_10577" sheetId="12" r:id="rId24"/>
+    <sheet name="RS_10554" sheetId="11" r:id="rId25"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId26"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId27"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId28"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId29"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId30"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId31"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId32"/>
+    <sheet name="RS_2389" sheetId="2" r:id="rId33"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId34"/>
   </sheets>
   <calcPr calcId="179020" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="177">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -332,6 +333,12 @@
   </si>
   <si>
     <t>IB1053915102018144235</t>
+  </si>
+  <si>
+    <t>SCN_GetPriceSCON_RS_10531</t>
+  </si>
+  <si>
+    <t>Product Name</t>
   </si>
   <si>
     <t>SCN_GetPrice_RS_10538</t>
@@ -760,10 +767,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1265,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1382,6 +1389,102 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9EC2A3-50A6-45AE-BF6E-1BAC3C249CC2}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{0780542D-ACE0-5A32-BFF3-888DF21E033C}">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1452,13 +1555,13 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>81</v>
@@ -1469,19 +1572,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1489,7 +1592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94480E05-B7FA-4DD5-89EE-C6E7F7328DF1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1520,7 +1623,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1531,10 +1634,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1609,7 +1712,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1632,7 +1735,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -1644,13 +1747,13 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1725,7 +1828,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -1734,7 +1837,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>61</v>
@@ -1742,7 +1845,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -1751,10 +1854,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1829,7 +1932,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1844,13 +1947,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
@@ -1862,7 +1965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -1932,7 +2035,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1949,13 +2052,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
@@ -1969,7 +2072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -2036,7 +2139,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2068,151 +2171,20 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
         <v>115</v>
       </c>
-      <c r="D3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -2328,462 +2300,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2846,7 +2366,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -2876,17 +2396,18 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>131</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -2909,11 +2430,463 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2987,24 +2960,16 @@
       <c r="D2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>136</v>
-      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="11"/>
+      <c r="N2" s="10"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -3013,30 +2978,21 @@
       <c r="T2" s="11"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>137</v>
+      <c r="A3" t="s">
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>142</v>
-      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -3057,10 +3013,10 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -3123,7 +3079,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3135,16 +3091,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3161,28 +3117,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3204,10 +3160,10 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -3282,16 +3238,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3314,22 +3270,22 @@
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3351,10 +3307,10 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -3429,16 +3385,16 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3461,22 +3417,22 @@
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3498,10 +3454,10 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -3564,7 +3520,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>22</v>
@@ -3576,23 +3532,23 @@
         <v>57</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -3602,28 +3558,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3784,6 +3740,153 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -3853,7 +3956,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -3865,10 +3968,10 @@
         <v>23</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -3887,22 +3990,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +4013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -3977,7 +4080,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -4011,7 +4114,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>27</v>
@@ -4023,10 +4126,10 @@
         <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4034,7 +4137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
@@ -4104,7 +4207,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -4113,19 +4216,19 @@
         <v>57</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4142,30 +4245,30 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>22</v>
@@ -4196,7 +4299,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>27</v>
@@ -4208,7 +4311,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="6"/>
@@ -4219,7 +4322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
commiting the data sheet
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_A591CCD61FB231D02A34A3D4F37152F691A5BD46" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="920" windowWidth="28800" windowHeight="16260" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16260" firstSheet="7" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -24,49 +23,47 @@
     <sheet name="RS_10585" sheetId="26" r:id="rId9"/>
     <sheet name="RS_10532" sheetId="25" r:id="rId10"/>
     <sheet name="RS_10539" sheetId="24" r:id="rId11"/>
-    <sheet name="RS_10531" sheetId="35" r:id="rId12"/>
-    <sheet name="RS_10538" sheetId="23" r:id="rId13"/>
-    <sheet name="RS_10536" sheetId="34" r:id="rId14"/>
-    <sheet name="RS_10586" sheetId="22" r:id="rId15"/>
-    <sheet name="RS_10566" sheetId="21" r:id="rId16"/>
-    <sheet name="RS_10550" sheetId="20" r:id="rId17"/>
-    <sheet name="RS_10544" sheetId="19" r:id="rId18"/>
-    <sheet name="RS_10556" sheetId="18" r:id="rId19"/>
-    <sheet name="RS_10557" sheetId="17" r:id="rId20"/>
-    <sheet name="RS_10580" sheetId="16" r:id="rId21"/>
-    <sheet name="RS_10579" sheetId="14" r:id="rId22"/>
-    <sheet name="RS_10578" sheetId="13" r:id="rId23"/>
-    <sheet name="RS_10577" sheetId="12" r:id="rId24"/>
-    <sheet name="RS_10554" sheetId="11" r:id="rId25"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId26"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId27"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId28"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId29"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId30"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId31"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId32"/>
-    <sheet name="RS_2389" sheetId="2" r:id="rId33"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId34"/>
+    <sheet name="RS_10538" sheetId="23" r:id="rId12"/>
+    <sheet name="RS_10586" sheetId="22" r:id="rId13"/>
+    <sheet name="RS_10566" sheetId="21" r:id="rId14"/>
+    <sheet name="RS_10550" sheetId="20" r:id="rId15"/>
+    <sheet name="RS_10544" sheetId="19" r:id="rId16"/>
+    <sheet name="RS_10556" sheetId="18" r:id="rId17"/>
+    <sheet name="RS_10557" sheetId="17" r:id="rId18"/>
+    <sheet name="RS_10580" sheetId="16" r:id="rId19"/>
+    <sheet name="RS_10579" sheetId="14" r:id="rId20"/>
+    <sheet name="RS_10578" sheetId="13" r:id="rId21"/>
+    <sheet name="RS_10577" sheetId="12" r:id="rId22"/>
+    <sheet name="RS_10554" sheetId="11" r:id="rId23"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId24"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId25"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId26"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId27"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId28"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId29"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId30"/>
+    <sheet name="RS_2389" sheetId="2" r:id="rId31"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="179020" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="175">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -110,69 +107,396 @@
     <t>Data13</t>
   </si>
   <si>
+    <t>RS_2389</t>
+  </si>
+  <si>
+    <t>ExploreSearch</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>ProductName1</t>
+  </si>
+  <si>
+    <t>ProductName2</t>
+  </si>
+  <si>
+    <t>ActivityType</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Case_RS_2389</t>
+  </si>
+  <si>
+    <t>Work Order Search 2</t>
+  </si>
+  <si>
+    <t>Record T&amp;M</t>
+  </si>
+  <si>
+    <t>BlueLake Men Watch</t>
+  </si>
+  <si>
+    <t>GE Product</t>
+  </si>
+  <si>
+    <t>Cleanup</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>RS_2389_checklist</t>
+  </si>
+  <si>
+    <t>ExploreChildSearch</t>
+  </si>
+  <si>
+    <t>ChecklistName</t>
+  </si>
+  <si>
+    <t>AUTOMATION SEARCH</t>
+  </si>
+  <si>
+    <t>Default title for Checklist</t>
+  </si>
+  <si>
+    <t>Work Orders</t>
+  </si>
+  <si>
+    <t>SFM_Auto_2372018162541</t>
+  </si>
+  <si>
+    <t>Scenario7_Checklist</t>
+  </si>
+  <si>
+    <t>ChecklistOpDocName</t>
+  </si>
+  <si>
+    <t>Data_Scenario7_Checklist</t>
+  </si>
+  <si>
+    <t>Scenario7_checklist</t>
+  </si>
+  <si>
+    <t>Scenario7OPDOC</t>
+  </si>
+  <si>
+    <t>SANITY5</t>
+  </si>
+  <si>
+    <t>IssueText</t>
+  </si>
+  <si>
+    <t>BillingType</t>
+  </si>
+  <si>
+    <t>DATA_SANITY5</t>
+  </si>
+  <si>
+    <t>SanityScenario5</t>
+  </si>
+  <si>
+    <t>Rule is billing type cannot be loan</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>SANITY6</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>DATA_SANITY6</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>lscenario6</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>RS_10552</t>
+  </si>
+  <si>
+    <t>SCN_RS_10552</t>
+  </si>
+  <si>
+    <t>RS_10552Sample</t>
+  </si>
+  <si>
+    <t>RS_10540</t>
+  </si>
+  <si>
+    <t>SCN_RS_10540</t>
+  </si>
+  <si>
+    <t>Installed Products</t>
+  </si>
+  <si>
+    <t>RS_10540_Process</t>
+  </si>
+  <si>
+    <t>RS_10541</t>
+  </si>
+  <si>
+    <t>SCN_RS_10541</t>
+  </si>
+  <si>
+    <t>RS_10542</t>
+  </si>
+  <si>
+    <t>SCN_RS_10542</t>
+  </si>
+  <si>
+    <t>RS-10554_mapping</t>
+  </si>
+  <si>
+    <t>Installed Product</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>EditProcessName</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_1_RS-10577_SOU</t>
+  </si>
+  <si>
+    <t>Manual_Checklist_Edit_WO_PROCESS</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_2_RS-10578_DVR</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_2_RS-10578_DVR</t>
+  </si>
+  <si>
+    <t>Manual_SCN_Checklist_2_RS-10578_ DVR</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_4_RS-10580_Sections</t>
+  </si>
+  <si>
+    <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
+  </si>
+  <si>
+    <t>ManualSCN_Checklist_4_RS-10580_Checklist_Sections</t>
+  </si>
+  <si>
+    <t>RS-10557_mapping</t>
+  </si>
+  <si>
+    <t>RS-10556_mapping</t>
+  </si>
+  <si>
+    <t>WorkOrder Number</t>
+  </si>
+  <si>
+    <t>Work Order</t>
+  </si>
+  <si>
+    <t>RS_10556_mapping</t>
+  </si>
+  <si>
+    <t>WO-00002089</t>
+  </si>
+  <si>
+    <t>SCN_SourceObjectUpdate_RS_10544</t>
+  </si>
+  <si>
+    <t>Data_SCN_SourceObjectUpdate_RS_10544</t>
+  </si>
+  <si>
+    <t>Manual_RS_10544_SOU</t>
+  </si>
+  <si>
+    <t>SCN_DVR_RS_10550</t>
+  </si>
+  <si>
+    <t>Data_SCN_DVR_RS_10550</t>
+  </si>
+  <si>
+    <t>AUTO_RS10550_DVR</t>
+  </si>
+  <si>
+    <t>RS_10566_Acc_Pro_History</t>
+  </si>
+  <si>
+    <t>ViewProcessNameAccPro</t>
+  </si>
+  <si>
+    <t>View Work Order</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_2_RS-10586</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_2_RS-10586</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_2_RS-10586snd</t>
+  </si>
+  <si>
+    <t>Manual_RS10586_ChecklistOPDOC</t>
+  </si>
+  <si>
+    <t>SCN_GetPrice_RS_10538</t>
+  </si>
+  <si>
+    <t>Work Order Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name </t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Installed Product Name</t>
+  </si>
+  <si>
+    <t>AutoA10538_Auto</t>
+  </si>
+  <si>
+    <t>SCN_GetPriceSCON_RS_10539</t>
+  </si>
+  <si>
+    <t>Product1 Name</t>
+  </si>
+  <si>
+    <t>Product2 Name</t>
+  </si>
+  <si>
+    <t>ServiceContract Name</t>
+  </si>
+  <si>
+    <t>WO-00003089</t>
+  </si>
+  <si>
+    <t>P1053951020181028521</t>
+  </si>
+  <si>
+    <t>P1053951020181028522</t>
+  </si>
+  <si>
+    <t>AutoScon5102018103339</t>
+  </si>
+  <si>
+    <t>AutoA10539_Auto</t>
+  </si>
+  <si>
+    <t>SCN_GetPriceNotCovered_RS_10532</t>
+  </si>
+  <si>
+    <t>WO-00002804</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_1_RS-10585</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_1_RS-10585</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10585_inProg</t>
+  </si>
+  <si>
+    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>ChecklistName_AllVersions</t>
+  </si>
+  <si>
+    <t>ChecklistName_FirstVersion</t>
+  </si>
+  <si>
+    <t>ChecklistName_LastVersion</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_allversions</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
+  </si>
+  <si>
+    <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
+    <t>RS_10565_Recent_Items</t>
+  </si>
+  <si>
+    <t>ViewProcessNameCustom</t>
+  </si>
+  <si>
+    <t>CreateNewCustomrecord</t>
+  </si>
+  <si>
+    <t>View Custom Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create New Custom Object </t>
+  </si>
+  <si>
+    <t>RS_10525_Calender_6</t>
+  </si>
+  <si>
+    <t>TechName</t>
+  </si>
+  <si>
+    <t>a240t000000GglLAAS</t>
+  </si>
+  <si>
+    <t>SCN_GetPrice_RS_10534</t>
+  </si>
+  <si>
+    <t>Work Order Number2</t>
+  </si>
+  <si>
+    <t>WO-00003104</t>
+  </si>
+  <si>
+    <t>WO-00003105</t>
+  </si>
+  <si>
     <t>SCN_GetPrice_RS_10537</t>
   </si>
   <si>
-    <t>Work Order Number</t>
-  </si>
-  <si>
-    <t>WO-00003264</t>
-  </si>
-  <si>
-    <t>SCN_GetPrice_RS_10534</t>
-  </si>
-  <si>
-    <t>Work Order Number2</t>
-  </si>
-  <si>
-    <t>WO-00003104</t>
-  </si>
-  <si>
-    <t>WO-00003105</t>
-  </si>
-  <si>
-    <t>RS_10525_Calender_6</t>
-  </si>
-  <si>
-    <t>ExploreSearch</t>
-  </si>
-  <si>
-    <t>ExploreChildSearch</t>
-  </si>
-  <si>
-    <t>ViewProcessNameCustom</t>
-  </si>
-  <si>
-    <t>WorkOrder Number</t>
-  </si>
-  <si>
-    <t>TechName</t>
-  </si>
-  <si>
-    <t>AUTOMATION SEARCH</t>
-  </si>
-  <si>
-    <t>Work Orders</t>
-  </si>
-  <si>
-    <t>View Custom Object</t>
-  </si>
-  <si>
-    <t>WO-00002848</t>
-  </si>
-  <si>
-    <t>a240t000000GglLAAS</t>
-  </si>
-  <si>
-    <t>RS_10565_Recent_Items</t>
-  </si>
-  <si>
-    <t>CreateNewCustomrecord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create New Custom Object </t>
-  </si>
-  <si>
     <t>RS_10511_Calender_1</t>
   </si>
   <si>
@@ -200,151 +524,16 @@
     <t>TechName2</t>
   </si>
   <si>
-    <t>WO-00002974</t>
-  </si>
-  <si>
-    <t>WO-00002975</t>
-  </si>
-  <si>
-    <t>WO-00002976</t>
-  </si>
-  <si>
-    <t>WO-00002978</t>
-  </si>
-  <si>
-    <t>WO-00002979</t>
-  </si>
-  <si>
-    <t>WO-00002980</t>
-  </si>
-  <si>
     <t>a240t000000L5IxAAK</t>
   </si>
   <si>
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
-    <t>WO-00003181</t>
-  </si>
-  <si>
-    <t>WO-00003182</t>
-  </si>
-  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
-    <t>WO-00003210</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
-    <t>ProcessName</t>
-  </si>
-  <si>
-    <t>ChecklistName_AllVersions</t>
-  </si>
-  <si>
-    <t>ChecklistName_FirstVersion</t>
-  </si>
-  <si>
-    <t>ChecklistName_LastVersion</t>
-  </si>
-  <si>
-    <t>EditProcessName</t>
-  </si>
-  <si>
-    <t>ChecklistOpDocName</t>
-  </si>
-  <si>
-    <t>Data_SCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
-    <t>Default title for Checklist</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_allversions</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
-  </si>
-  <si>
-    <t>Manual_Checklist_Edit_WO_PROCESS</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_1_RS-10585</t>
-  </si>
-  <si>
-    <t>ChecklistName</t>
-  </si>
-  <si>
-    <t>Data_SCN_ChecklistOPDOC_1_RS-10585</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10585_inProg</t>
-  </si>
-  <si>
-    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
-  </si>
-  <si>
-    <t>SCN_GetPriceNotCovered_RS_10532</t>
-  </si>
-  <si>
-    <t>WO-00002804</t>
-  </si>
-  <si>
-    <t>SCN_GetPriceSCON_RS_10539</t>
-  </si>
-  <si>
-    <t>Product1 Name</t>
-  </si>
-  <si>
-    <t>Product2 Name</t>
-  </si>
-  <si>
-    <t>ServiceContract Name</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Installed Product Name</t>
-  </si>
-  <si>
-    <t>WO-00003261</t>
-  </si>
-  <si>
-    <t>P10539121020181328351</t>
-  </si>
-  <si>
-    <t>P10539121020181328352</t>
-  </si>
-  <si>
-    <t>AutoScon12102018133355</t>
-  </si>
-  <si>
-    <t>Auto_1053912102018133339</t>
-  </si>
-  <si>
-    <t>IB1053915102018144235</t>
-  </si>
-  <si>
-    <t>SCN_GetPriceSCON_RS_10531</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>SCN_GetPrice_RS_10538</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Name </t>
+    <t>WO-00003237</t>
   </si>
   <si>
     <t>WO-00003256</t>
@@ -353,264 +542,59 @@
     <t>P1053812102018105539</t>
   </si>
   <si>
-    <t>AutoA10538_Auto</t>
-  </si>
-  <si>
     <t>IB1053812102018105541</t>
   </si>
   <si>
-    <t>SCN_GetPrice_RS_10536</t>
-  </si>
-  <si>
-    <t>WO-00003370</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_2_RS-10586</t>
-  </si>
-  <si>
-    <t>Data_SCN_ChecklistOPDOC_2_RS-10586</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_2_RS-10586snd</t>
-  </si>
-  <si>
-    <t>Manual_RS10586_ChecklistOPDOC</t>
-  </si>
-  <si>
-    <t>RS_10566_Acc_Pro_History</t>
-  </si>
-  <si>
-    <t>ViewProcessNameAccPro</t>
-  </si>
-  <si>
-    <t>View Work Order</t>
-  </si>
-  <si>
-    <t>SCN_DVR_RS_10550</t>
-  </si>
-  <si>
-    <t>Data_SCN_DVR_RS_10550</t>
-  </si>
-  <si>
-    <t>AUTO_RS10550_DVR</t>
-  </si>
-  <si>
-    <t>SCN_SourceObjectUpdate_RS_10544</t>
-  </si>
-  <si>
-    <t>Data_SCN_SourceObjectUpdate_RS_10544</t>
-  </si>
-  <si>
-    <t>Manual_RS_10544_SOU</t>
-  </si>
-  <si>
-    <t>RS-10556_mapping</t>
-  </si>
-  <si>
-    <t>Work Order</t>
-  </si>
-  <si>
-    <t>RS_10556_mapping</t>
-  </si>
-  <si>
-    <t>WO-00002089</t>
-  </si>
-  <si>
-    <t>RS-10557_mapping</t>
-  </si>
-  <si>
-    <t>Installed Product</t>
-  </si>
-  <si>
-    <t>RS_10557_592018205141</t>
-  </si>
-  <si>
-    <t>SCN_Checklist_4_RS-10580_Sections</t>
-  </si>
-  <si>
-    <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
-  </si>
-  <si>
-    <t>ManualSCN_Checklist_4_RS-10580_Checklist_Sections</t>
-  </si>
-  <si>
-    <t>SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
-  </si>
-  <si>
-    <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
-  </si>
-  <si>
-    <t>ManualSCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
-  </si>
-  <si>
-    <t>SCN_Checklist_2_RS-10578_DVR</t>
-  </si>
-  <si>
-    <t>Data_SCN_Checklist_2_RS-10578_DVR</t>
-  </si>
-  <si>
-    <t>Manual_SCN_Checklist_2_RS-10578_ DVR</t>
-  </si>
-  <si>
-    <t>SCN_Checklist_1_RS-10577_SOU</t>
-  </si>
-  <si>
-    <t>Data_SCN_Checklist_1_RS-10577_SOU</t>
-  </si>
-  <si>
-    <t>ManualSCN_Checklist_1_RS-10577_SOU</t>
-  </si>
-  <si>
-    <t>Scenario7OPDOC</t>
-  </si>
-  <si>
-    <t>RS-10554_mapping</t>
-  </si>
-  <si>
-    <t>RS_10554_7920189427</t>
-  </si>
-  <si>
-    <t>RS_10542</t>
-  </si>
-  <si>
-    <t>IssueText</t>
-  </si>
-  <si>
-    <t>OrderStatus</t>
-  </si>
-  <si>
-    <t>BillingType</t>
-  </si>
-  <si>
-    <t>ProductName1</t>
-  </si>
-  <si>
-    <t>SCN_RS_10542</t>
-  </si>
-  <si>
-    <t>Installed Products</t>
-  </si>
-  <si>
-    <t>RS_10540_Process</t>
-  </si>
-  <si>
-    <t>Loan</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>RS_10541</t>
-  </si>
-  <si>
-    <t>SCN_RS_10541</t>
-  </si>
-  <si>
-    <t>RS_10540</t>
-  </si>
-  <si>
-    <t>SCN_RS_10540</t>
-  </si>
-  <si>
-    <t>RS_10552</t>
-  </si>
-  <si>
-    <t>SCN_RS_10552</t>
-  </si>
-  <si>
-    <t>RS_10552Sample</t>
-  </si>
-  <si>
-    <t>SANITY6</t>
-  </si>
-  <si>
-    <t>DATA_SANITY6</t>
-  </si>
-  <si>
-    <t>Cases</t>
-  </si>
-  <si>
-    <t>lscenario6</t>
-  </si>
-  <si>
-    <t>SANITY5</t>
-  </si>
-  <si>
-    <t>DATA_SANITY5</t>
-  </si>
-  <si>
-    <t>SanityScenario5</t>
-  </si>
-  <si>
-    <t>Rule is billing type cannot be loan</t>
-  </si>
-  <si>
-    <t>Scenario7_Checklist</t>
-  </si>
-  <si>
-    <t>Data_Scenario7_Checklist</t>
-  </si>
-  <si>
-    <t>Scenario7_checklist</t>
-  </si>
-  <si>
-    <t>RS_2389</t>
-  </si>
-  <si>
-    <t>ProductName2</t>
-  </si>
-  <si>
-    <t>ActivityType</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Case_RS_2389</t>
-  </si>
-  <si>
-    <t>Work Order Search 2</t>
-  </si>
-  <si>
-    <t>Record T&amp;M</t>
-  </si>
-  <si>
-    <t>BlueLake Men Watch</t>
-  </si>
-  <si>
-    <t>GE Product</t>
-  </si>
-  <si>
-    <t>Cleanup</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>RS_2389_checklist</t>
-  </si>
-  <si>
-    <t>SFM_Auto_2372018162541</t>
-  </si>
-  <si>
-    <t>WO-00003389</t>
-  </si>
-  <si>
-    <t>P1053117102018101621</t>
+    <t>RS_10554_field_mapping</t>
+  </si>
+  <si>
+    <t>RS_10557_Child_Mapping</t>
+  </si>
+  <si>
+    <t>Salesforceuser</t>
+  </si>
+  <si>
+    <t>0050t000001PqX7AAK</t>
+  </si>
+  <si>
+    <t>WO-00003335</t>
+  </si>
+  <si>
+    <t>WO-00003336</t>
+  </si>
+  <si>
+    <t>WO-00003337</t>
+  </si>
+  <si>
+    <t>WO-00003338</t>
+  </si>
+  <si>
+    <t>WO-00003339</t>
+  </si>
+  <si>
+    <t>WO-00003340</t>
+  </si>
+  <si>
+    <t>WO-00003346</t>
+  </si>
+  <si>
+    <t>WO-00003347</t>
+  </si>
+  <si>
+    <t>WO-00003348</t>
+  </si>
+  <si>
+    <t>WO-00003349</t>
+  </si>
+  <si>
+    <t>WO-00003361</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,7 +732,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -772,12 +756,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1090,27 +1075,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1165,21 +1150,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1190,16 +1175,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1254,20 +1239,20 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1276,20 +1261,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="6" max="6" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="51.7109375" collapsed="true"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1344,50 +1325,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1396,22 +1371,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9EC2A3-50A6-45AE-BF6E-1BAC3C249CC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{0780542D-ACE0-5A32-BFF3-888DF21E033C}">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1466,30 +1439,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:19">
+        <v>103</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1498,20 +1479,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FF0BDA26-1AD6-5648-BD9A-E01AA4DDCA7C}">
-      <selection sqref="A1:E1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1566,38 +1543,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>95</v>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1606,18 +1595,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94480E05-B7FA-4DD5-89EE-C6E7F7328DF1}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{62312496-B7DB-5A1E-BE5B-04E292D686FF}"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,24 +1624,77 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
+      <c r="C2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1659,16 +1703,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C67EF94B-0B3B-5838-830C-E3A509766221}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1723,51 +1767,35 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>102</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1775,16 +1803,19 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{274F5AE0-5452-572F-8038-C13FFDA59D49}">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1839,38 +1870,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>103</v>
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1879,16 +1910,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{33642244-9AC9-5136-AF77-195C889548CE}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1943,228 +1974,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D624DF06-3800-545C-AC8D-BADC89115800}">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{11A3ACCB-1F19-5AC9-A611-4158731A345D}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -2182,21 +2006,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2220,17 +2044,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S3"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,110 +2113,18 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2407,18 +2143,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2443,20 +2179,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2511,44 +2247,359 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2557,19 +2608,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2624,44 +2672,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>124</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2670,16 +2724,21 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2734,244 +2793,18 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2990,18 +2823,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3025,17 +2858,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3090,30 +2923,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3128,30 +2961,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3172,17 +3005,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3237,30 +3070,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>145</v>
+        <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3275,30 +3108,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3319,17 +3152,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3384,30 +3217,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3422,30 +3255,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3466,17 +3299,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3531,30 +3364,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>149</v>
+        <v>55</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3569,30 +3402,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>151</v>
+        <v>57</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3613,17 +3446,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3678,25 +3511,303 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>26</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -3712,24 +3823,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" t="s">
+        <v>138</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -3753,16 +3861,16 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3817,174 +3925,24 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:T3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{EE242A16-C6B8-5192-B120-522BC795EE76}">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>135</v>
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4001,24 +3959,24 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>158</v>
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>159</v>
+        <v>39</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4026,17 +3984,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:T3"/>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7075697D-051A-5480-9A35-AA80E904E1A1}">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4091,27 +4052,31 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -4125,175 +4090,44 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C7A11F4D-6E51-5B1A-9CF2-8FFD2B06F078}">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -4310,21 +4144,21 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="6"/>
@@ -4335,29 +4169,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D979DC6D-665A-5B40-B235-9A07D260EAB6}"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4412,21 +4253,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4444,21 +4285,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -4482,16 +4323,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4546,41 +4395,43 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>42</v>
+        <v>151</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="10"/>
+        <v>152</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="11"/>
@@ -4590,41 +4441,43 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="8"/>
+        <v>165</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>163</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -4641,16 +4494,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4705,21 +4562,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4737,22 +4594,28 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>53</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -4770,16 +4633,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4834,21 +4700,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4866,19 +4732,28 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>55</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -4896,16 +4771,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4960,62 +4835,62 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -5024,16 +4899,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5088,50 +4963,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes of the code RS_10531
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="183">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -603,6 +603,18 @@
   </si>
   <si>
     <t>P1053117102018101621</t>
+  </si>
+  <si>
+    <t>WO-00003396</t>
+  </si>
+  <si>
+    <t>P1053117102018142358</t>
+  </si>
+  <si>
+    <t>WO-00003397</t>
+  </si>
+  <si>
+    <t>P1053117102018143218</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1498,10 @@
         <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing TestData file and inprogress 10569
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27B723D2-FBC7-3043-AAAA-D8E7F8311B5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157271E2-6EA9-6541-B0C8-37C7AA1FB683}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2820" windowWidth="28800" windowHeight="16260" firstSheet="29" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="28800" windowHeight="16260" firstSheet="23" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -49,17 +49,12 @@
     <sheet name="SANITY5" sheetId="5" r:id="rId34"/>
     <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId35"/>
     <sheet name="RS_2389" sheetId="2" r:id="rId36"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId37"/>
+    <sheet name="RS_10569" sheetId="15" r:id="rId37"/>
   </sheets>
-  <calcPr calcId="179020" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -69,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="195">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -648,14 +643,19 @@
   </si>
   <si>
     <t>WO-00003612</t>
+  </si>
+  <si>
+    <t>SCN_ScheduledDataSync_RS_10569</t>
+  </si>
+  <si>
+    <t>DATA_SCN_ScheduledDataSync_RS_10569</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,24 +1148,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1248,13 +1248,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>74</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>76</v>
       </c>
@@ -1364,13 +1364,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1450,17 +1450,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1570,17 +1570,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565C9F66-DE32-407C-8352-EDC4D209770F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{0BAA6026-4B65-5428-B09E-8D45E4A3F823}">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>93</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1613,18 +1613,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0868B021-31A6-41FF-9123-26E8DE5E1E5C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{D38B9E41-2F26-5DD1-8A39-56CE88C41251}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="50.140625" collapsed="true"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1666,17 +1666,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FF0BDA26-1AD6-5648-BD9A-E01AA4DDCA7C}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1774,13 +1774,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C67EF94B-0B3B-5838-830C-E3A509766221}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>105</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>106</v>
       </c>
@@ -1890,17 +1890,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{274F5AE0-5452-572F-8038-C13FFDA59D49}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>109</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>109</v>
       </c>
@@ -1998,13 +1998,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{33642244-9AC9-5136-AF77-195C889548CE}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>112</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>113</v>
       </c>
@@ -2098,16 +2098,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D624DF06-3800-545C-AC8D-BADC89115800}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>116</v>
       </c>
@@ -2205,13 +2205,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2297,13 +2297,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{11A3ACCB-1F19-5AC9-A611-4158731A345D}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2358,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>118</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2432,17 +2432,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>122</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -2567,16 +2567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>125</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>126</v>
       </c>
@@ -2680,16 +2680,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>128</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>129</v>
       </c>
@@ -2793,13 +2793,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>131</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>132</v>
       </c>
@@ -2903,16 +2903,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.7109375" collapsed="false"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>134</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>135</v>
       </c>
@@ -3022,18 +3022,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>138</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -3157,13 +3157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3218,7 +3218,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>140</v>
       </c>
@@ -3256,7 +3256,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>145</v>
       </c>
@@ -3304,13 +3304,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3365,7 +3365,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>151</v>
       </c>
@@ -3403,7 +3403,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>152</v>
       </c>
@@ -3451,16 +3451,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3515,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>153</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>154</v>
       </c>
@@ -3601,18 +3601,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F29D048-4285-409C-863D-4F3066F7E9FF}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{944A36CB-ED4E-58DF-8362-89F5B188B9CE}">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="false"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -3638,7 +3638,7 @@
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3655,22 +3655,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3687A34-96AE-FD4C-86A6-B2E37D5941C4}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{8CB1866D-8B2D-5826-87E1-D92C6E17B3B4}">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.7109375" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="31.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="false"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3725,7 +3725,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>155</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>159</v>
       </c>
@@ -3781,17 +3781,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A51DDAF-FBC4-F949-9577-B391C7BC74DF}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{612FF438-05BC-5BC6-9544-64173AA0545C}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="22.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="26.85546875" collapsed="false"/>
+    <col min="2" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3846,7 +3846,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>161</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>162</v>
       </c>
@@ -3916,13 +3916,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3977,7 +3977,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>164</v>
       </c>
@@ -4015,7 +4015,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>165</v>
       </c>
@@ -4063,13 +4063,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4124,7 +4124,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>167</v>
       </c>
@@ -4162,7 +4162,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>168</v>
       </c>
@@ -4210,16 +4210,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{EE242A16-C6B8-5192-B120-522BC795EE76}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>172</v>
       </c>
@@ -4337,13 +4337,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7075697D-051A-5480-9A35-AA80E904E1A1}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4398,7 +4398,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>175</v>
       </c>
@@ -4432,7 +4432,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>176</v>
       </c>
@@ -4461,16 +4461,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C7A11F4D-6E51-5B1A-9CF2-8FFD2B06F078}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4525,7 +4525,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>178</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>190</v>
       </c>
@@ -4617,7 +4617,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -4644,12 +4644,108 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D979DC6D-665A-5B40-B235-9A07D260EAB6}"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4658,19 +4754,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4725,7 +4821,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
@@ -4757,7 +4853,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4798,20 +4894,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4866,7 +4962,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -4898,7 +4994,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4939,21 +5035,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5008,7 +5104,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -5054,7 +5150,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -5110,17 +5206,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5175,7 +5271,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>54</v>
       </c>
@@ -5207,7 +5303,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -5243,16 +5339,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5307,7 +5403,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>57</v>
       </c>
@@ -5339,7 +5435,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -5375,13 +5471,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5436,7 +5532,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
@@ -5465,7 +5561,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
pushing test data and script for 10574
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,57 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDE3574-6D56-9B4D-8639-6113F90DB794}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="28800" windowHeight="16260" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="33800" yWindow="2960" windowWidth="28800" windowHeight="16260" firstSheet="24" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
     <sheet name="RS_10534" sheetId="30" r:id="rId2"/>
     <sheet name="RS_10533" sheetId="38" r:id="rId3"/>
-    <sheet name="RS_10514" sheetId="39" r:id="rId4"/>
-    <sheet name="RS_10525" sheetId="29" r:id="rId5"/>
-    <sheet name="RS_10565" sheetId="28" r:id="rId6"/>
-    <sheet name="RS_10511" sheetId="31" r:id="rId7"/>
-    <sheet name="RS_10513" sheetId="32" r:id="rId8"/>
-    <sheet name="RS_11859" sheetId="33" r:id="rId9"/>
-    <sheet name="RS_10587" sheetId="27" r:id="rId10"/>
-    <sheet name="RS_10585" sheetId="26" r:id="rId11"/>
-    <sheet name="RS_10532" sheetId="25" r:id="rId12"/>
-    <sheet name="RS_10539" sheetId="24" r:id="rId13"/>
-    <sheet name="RS_10536" sheetId="34" r:id="rId14"/>
-    <sheet name="RS_10531" sheetId="35" r:id="rId15"/>
-    <sheet name="RS_10538" sheetId="23" r:id="rId16"/>
-    <sheet name="RS_10586" sheetId="22" r:id="rId17"/>
-    <sheet name="RS_10566" sheetId="21" r:id="rId18"/>
-    <sheet name="RS_10550" sheetId="20" r:id="rId19"/>
-    <sheet name="RS_10544" sheetId="19" r:id="rId20"/>
-    <sheet name="RS_10556" sheetId="18" r:id="rId21"/>
-    <sheet name="RS_10557" sheetId="17" r:id="rId22"/>
-    <sheet name="RS_10580" sheetId="16" r:id="rId23"/>
-    <sheet name="RS_10579" sheetId="14" r:id="rId24"/>
-    <sheet name="RS_10578" sheetId="13" r:id="rId25"/>
-    <sheet name="RS_10577" sheetId="12" r:id="rId26"/>
-    <sheet name="RS_10554" sheetId="11" r:id="rId27"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId28"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId29"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId30"/>
-    <sheet name="RS_10571" sheetId="36" r:id="rId31"/>
-    <sheet name="RS_10562" sheetId="37" r:id="rId32"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId33"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId34"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId35"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId36"/>
+    <sheet name="RS_10525" sheetId="29" r:id="rId4"/>
+    <sheet name="RS_10565" sheetId="28" r:id="rId5"/>
+    <sheet name="RS_10511" sheetId="31" r:id="rId6"/>
+    <sheet name="RS_10513" sheetId="32" r:id="rId7"/>
+    <sheet name="RS_11859" sheetId="33" r:id="rId8"/>
+    <sheet name="RS_10587" sheetId="27" r:id="rId9"/>
+    <sheet name="RS_10585" sheetId="26" r:id="rId10"/>
+    <sheet name="RS_10532" sheetId="25" r:id="rId11"/>
+    <sheet name="RS_10539" sheetId="24" r:id="rId12"/>
+    <sheet name="RS_10536" sheetId="34" r:id="rId13"/>
+    <sheet name="RS_10531" sheetId="35" r:id="rId14"/>
+    <sheet name="RS_10538" sheetId="23" r:id="rId15"/>
+    <sheet name="RS_10586" sheetId="22" r:id="rId16"/>
+    <sheet name="RS_10566" sheetId="21" r:id="rId17"/>
+    <sheet name="RS_10550" sheetId="20" r:id="rId18"/>
+    <sheet name="RS_10544" sheetId="19" r:id="rId19"/>
+    <sheet name="RS_10556" sheetId="18" r:id="rId20"/>
+    <sheet name="RS_10557" sheetId="17" r:id="rId21"/>
+    <sheet name="RS_10580" sheetId="16" r:id="rId22"/>
+    <sheet name="RS_10579" sheetId="14" r:id="rId23"/>
+    <sheet name="RS_10578" sheetId="13" r:id="rId24"/>
+    <sheet name="RS_10577" sheetId="12" r:id="rId25"/>
+    <sheet name="RS_10554" sheetId="11" r:id="rId26"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId27"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId28"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId29"/>
+    <sheet name="RS_10571" sheetId="36" r:id="rId30"/>
+    <sheet name="RS_10562" sheetId="37" r:id="rId31"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId32"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId33"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId34"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId35"/>
+    <sheet name="RS_10574" sheetId="40" r:id="rId36"/>
     <sheet name="RS_2389" sheetId="2" r:id="rId37"/>
     <sheet name="RS_10569" sheetId="15" r:id="rId38"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,17 +60,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="198">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -659,16 +655,16 @@
     <t>P105332610201816037</t>
   </si>
   <si>
-    <t>Auto_Tech_Service_user1</t>
-  </si>
-  <si>
-    <t>RS_10514_Calender_4</t>
+    <t>SCN_Creating_Editing_RS_10574</t>
+  </si>
+  <si>
+    <t>Data_SCN_Creating_Editing_RS_10574</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1159,7 +1155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
@@ -1259,7 +1255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1325,7 +1321,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -1337,24 +1333,18 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -1366,19 +1356,13 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1387,123 +1371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1588,8 +1456,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1708,11 +1576,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565C9F66-DE32-407C-8352-EDC4D209770F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
@@ -1751,11 +1619,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0868B021-31A6-41FF-9123-26E8DE5E1E5C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1804,8 +1672,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1912,8 +1780,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2028,8 +1896,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2136,8 +2004,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2236,100 +2104,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2435,8 +2211,100 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2570,11 +2438,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A2" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -2705,12 +2573,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2818,8 +2686,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2931,8 +2799,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3041,8 +2909,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3160,8 +3028,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3295,8 +3163,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3442,8 +3310,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3589,11 +3457,161 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F29D048-4285-409C-863D-4F3066F7E9FF}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3649,160 +3667,10 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3687A34-96AE-FD4C-86A6-B2E37D5941C4}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3924,12 +3792,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A51DDAF-FBC4-F949-9577-B391C7BC74DF}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4059,8 +3927,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4206,12 +4074,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4353,8 +4221,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4480,15 +4348,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -4604,8 +4475,87 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A487FAA-A3CC-3948-ADB8-95541386AC0F}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4790,7 +4740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4898,19 +4848,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showRuler="0" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4924,10 +4874,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -4970,16 +4920,20 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -4998,135 +4952,6 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
@@ -5162,8 +4987,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5303,12 +5128,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5474,8 +5299,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5607,8 +5432,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5737,4 +5562,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pushing changes of the Regression stabalization.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="215">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -704,6 +704,12 @@
   </si>
   <si>
     <t>P105339112018153027</t>
+  </si>
+  <si>
+    <t>WO-00004265</t>
+  </si>
+  <si>
+    <t>P105339112018164153</t>
   </si>
 </sst>
 </file>
@@ -3701,10 +3707,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing changes for 10577
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF48088E-8C09-F14F-8A11-FE48241B5350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="16260" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16260" firstSheet="14" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -53,7 +54,7 @@
     <sheet name="RS_2389" sheetId="2" r:id="rId39"/>
     <sheet name="RS_10569" sheetId="15" r:id="rId40"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,11 +62,6 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -448,9 +444,6 @@
     <t>Data_SCN_Checklist_1_RS-10577_SOU</t>
   </si>
   <si>
-    <t>ManualSCN_Checklist_1_RS-10577_SOU</t>
-  </si>
-  <si>
     <t>Scenario7OPDOC</t>
   </si>
   <si>
@@ -710,12 +703,15 @@
   </si>
   <si>
     <t>WO-00004368</t>
+  </si>
+  <si>
+    <t>AUTO_EDIT_WORKORDER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1206,7 +1202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
@@ -1306,10 +1302,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1417,10 +1413,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>211</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1439,7 +1435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1549,10 +1545,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" t="s">
         <v>204</v>
-      </c>
-      <c r="E3" t="s">
-        <v>205</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1571,7 +1567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1699,7 +1695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1815,7 +1811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1901,7 +1897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2021,7 +2017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2064,7 +2060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2117,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2225,7 +2221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2341,7 +2337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2433,7 +2429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2541,7 +2537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2641,7 +2637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2748,7 +2744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2883,7 +2879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3018,7 +3014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3131,7 +3127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3244,7 +3240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3354,16 +3350,19 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3458,13 +3457,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>62</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3473,7 +3472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3544,7 +3543,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3574,7 +3573,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3583,7 +3582,7 @@
         <v>112</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3608,7 +3607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3655,10 +3654,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
         <v>183</v>
-      </c>
-      <c r="C3" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3667,7 +3666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3733,7 +3732,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3745,16 +3744,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3771,28 +3770,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3814,7 +3813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3880,7 +3879,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3892,16 +3891,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3918,28 +3917,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3961,7 +3960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4030,7 +4029,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4042,16 +4041,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4068,28 +4067,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4111,7 +4110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
@@ -4186,7 +4185,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4198,18 +4197,18 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4224,7 +4223,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4237,7 +4236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4307,7 +4306,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4337,7 +4336,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4346,7 +4345,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4372,7 +4371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4438,7 +4437,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4450,16 +4449,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4476,7 +4475,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4485,19 +4484,19 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4519,7 +4518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4585,7 +4584,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4597,16 +4596,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4623,28 +4622,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="E3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4666,7 +4665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4735,7 +4734,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4747,10 +4746,10 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4769,22 +4768,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4793,7 +4792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4859,7 +4858,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4893,7 +4892,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4905,10 +4904,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4917,7 +4916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4986,7 +4985,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4995,19 +4994,19 @@
         <v>51</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -5024,30 +5023,30 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
         <v>172</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>173</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>174</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>175</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>176</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>177</v>
-      </c>
-      <c r="G3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>24</v>
@@ -5078,7 +5077,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>28</v>
@@ -5090,7 +5089,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="6"/>
@@ -5102,7 +5101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5174,7 +5173,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>44</v>
@@ -5202,10 +5201,10 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>47</v>
@@ -5227,7 +5226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5297,7 +5296,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -5314,7 +5313,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5335,7 +5334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5448,7 +5447,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -5475,7 +5474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5616,7 +5615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5745,22 +5744,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>199</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>200</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>201</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>202</v>
-      </c>
-      <c r="I3" t="s">
-        <v>203</v>
       </c>
       <c r="J3" t="s">
         <v>30</v>
@@ -5787,7 +5786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5860,7 +5859,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -5878,7 +5877,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -5896,7 +5895,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -5905,16 +5904,16 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>208</v>
-      </c>
-      <c r="G3" t="s">
-        <v>209</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -5932,7 +5931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -6005,7 +6004,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -6023,13 +6022,13 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6045,7 +6044,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -6054,22 +6053,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>193</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>194</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>195</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>196</v>
-      </c>
-      <c r="I3" t="s">
-        <v>197</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
changes from tap to click and updates TestData File scenario2 is incorrect
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F3E3265A-02E0-8541-A98F-25ECADB86718}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146FF3ED-461B-9749-8888-9D5EEDA45B63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16260" firstSheet="19" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16260" firstSheet="25" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -42,18 +42,17 @@
     <sheet name="RS_10578" sheetId="13" r:id="rId27"/>
     <sheet name="RS_10577" sheetId="12" r:id="rId28"/>
     <sheet name="RS_10554" sheetId="11" r:id="rId29"/>
-    <sheet name="RS_10543" sheetId="42" r:id="rId30"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId31"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId32"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId33"/>
-    <sheet name="RS_10571" sheetId="36" r:id="rId34"/>
-    <sheet name="RS_10562" sheetId="37" r:id="rId35"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId36"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId37"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId38"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId39"/>
-    <sheet name="RS_2389" sheetId="2" r:id="rId40"/>
-    <sheet name="RS_10569" sheetId="15" r:id="rId41"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId30"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId31"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId32"/>
+    <sheet name="RS_10571" sheetId="36" r:id="rId33"/>
+    <sheet name="RS_10562" sheetId="37" r:id="rId34"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId35"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId36"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId37"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId38"/>
+    <sheet name="RS_2389" sheetId="2" r:id="rId39"/>
+    <sheet name="RS_10569" sheetId="15" r:id="rId40"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="201">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -436,9 +435,6 @@
     <t>Data_SCN_Checklist_2_RS-10578_DVR</t>
   </si>
   <si>
-    <t>Manual_SCN_Checklist_2_RS-10578_ DVR</t>
-  </si>
-  <si>
     <t>SCN_Checklist_1_RS-10577_SOU</t>
   </si>
   <si>
@@ -568,42 +564,6 @@
     <t>Scenario7_checklist</t>
   </si>
   <si>
-    <t>RS_2389</t>
-  </si>
-  <si>
-    <t>ProductName2</t>
-  </si>
-  <si>
-    <t>ActivityType</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Case_RS_2389</t>
-  </si>
-  <si>
-    <t>Work Order Search 2</t>
-  </si>
-  <si>
-    <t>Record T&amp;M</t>
-  </si>
-  <si>
-    <t>BlueLake Men Watch</t>
-  </si>
-  <si>
-    <t>GE Product</t>
-  </si>
-  <si>
-    <t>Cleanup</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>RS_2389_checklist</t>
   </si>
   <si>
@@ -709,16 +669,7 @@
     <t>AUTO_EDIT_WORKORDER</t>
   </si>
   <si>
-    <t>RS_10543</t>
-  </si>
-  <si>
-    <t>SCN_RS_10543</t>
-  </si>
-  <si>
-    <t>RS_10543 SFM Search for Multi Page View</t>
-  </si>
-  <si>
-    <t>Empowerment</t>
+    <t>Auto_10578_ChecklistDVR</t>
   </si>
 </sst>
 </file>
@@ -1426,10 +1377,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1558,10 +1509,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -3257,10 +3208,15 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -3351,10 +3307,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3366,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3435,7 +3391,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -3458,7 +3414,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3470,13 +3426,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3556,7 +3512,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3586,7 +3542,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3595,7 +3551,7 @@
         <v>112</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3667,10 +3623,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3679,141 +3635,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26C13FA-F956-6341-A30E-059B800D1E0B}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -3880,7 +3701,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3892,16 +3713,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3918,28 +3739,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3960,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4027,7 +3848,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4039,16 +3860,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4065,28 +3886,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4107,7 +3928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4177,7 +3998,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4189,16 +4010,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4215,28 +4036,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4257,7 +4078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -4333,7 +4154,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4345,18 +4166,18 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4371,7 +4192,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4383,7 +4204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4454,7 +4275,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4484,7 +4305,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4493,7 +4314,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4518,7 +4339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4585,7 +4406,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4597,16 +4418,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4623,7 +4444,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4632,19 +4453,19 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4665,7 +4486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4732,7 +4553,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4744,16 +4565,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4770,28 +4591,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>158</v>
-      </c>
       <c r="E3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4812,7 +4633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -4882,7 +4703,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4894,10 +4715,10 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4916,22 +4737,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4939,15 +4760,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -5006,7 +4834,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -5040,7 +4868,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5052,11 +4880,139 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>125</v>
-      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5136,7 +5092,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>44</v>
@@ -5164,10 +5120,10 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>47</v>
@@ -5189,191 +5145,6 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -5444,7 +5215,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -5461,7 +5232,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5595,7 +5366,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -5892,22 +5663,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="J3" t="s">
         <v>30</v>
@@ -6007,7 +5778,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -6025,7 +5796,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -6043,7 +5814,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -6052,16 +5823,16 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="F3" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6152,7 +5923,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -6170,13 +5941,13 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6192,7 +5963,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -6201,22 +5972,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="I3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
pushing testdata for 10584
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{48B0361B-319C-1843-AA2C-A46D2D10852E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0682317-47BB-6444-9FED-27490CAF625E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16260" firstSheet="19" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="12" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -38,22 +38,23 @@
     <sheet name="RS_10556" sheetId="18" r:id="rId23"/>
     <sheet name="RS_10557" sheetId="17" r:id="rId24"/>
     <sheet name="RS_10580" sheetId="16" r:id="rId25"/>
-    <sheet name="RS_10579" sheetId="14" r:id="rId26"/>
-    <sheet name="RS_10578" sheetId="13" r:id="rId27"/>
-    <sheet name="RS_10577" sheetId="12" r:id="rId28"/>
-    <sheet name="RS_10554" sheetId="11" r:id="rId29"/>
-    <sheet name="RS_10543" sheetId="42" r:id="rId30"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId31"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId32"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId33"/>
-    <sheet name="RS_10571" sheetId="36" r:id="rId34"/>
-    <sheet name="RS_10562" sheetId="37" r:id="rId35"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId36"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId37"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId38"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId39"/>
-    <sheet name="RS_2389" sheetId="2" r:id="rId40"/>
-    <sheet name="RS_10569" sheetId="15" r:id="rId41"/>
+    <sheet name="RS_10584" sheetId="43" r:id="rId26"/>
+    <sheet name="RS_10579" sheetId="14" r:id="rId27"/>
+    <sheet name="RS_10578" sheetId="13" r:id="rId28"/>
+    <sheet name="RS_10577" sheetId="12" r:id="rId29"/>
+    <sheet name="RS_10554" sheetId="11" r:id="rId30"/>
+    <sheet name="RS_10543" sheetId="42" r:id="rId31"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId32"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId33"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId34"/>
+    <sheet name="RS_10571" sheetId="36" r:id="rId35"/>
+    <sheet name="RS_10562" sheetId="37" r:id="rId36"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId37"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId38"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId39"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId40"/>
+    <sheet name="RS_2389" sheetId="2" r:id="rId41"/>
+    <sheet name="RS_10569" sheetId="15" r:id="rId42"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="207">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -256,9 +257,6 @@
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
   </si>
   <si>
-    <t>Manual_Checklist_Edit_WO_PROCESS</t>
-  </si>
-  <si>
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
@@ -683,6 +681,15 @@
   </si>
   <si>
     <t>Empowerment</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistAttachment_RS-10584</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistAttachment_RS_10584</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_Attachment</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1397,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>197</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>198</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1522,10 +1529,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
         <v>190</v>
-      </c>
-      <c r="E3" t="s">
-        <v>191</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1548,7 +1555,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,10 +1667,10 @@
         <v>61</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" t="s">
         <v>62</v>
-      </c>
-      <c r="I3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1683,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1738,7 +1745,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -1750,7 +1757,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>55</v>
@@ -1761,7 +1768,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -1773,13 +1780,13 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
         <v>67</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1854,7 +1861,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1862,10 +1869,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1944,48 +1951,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2024,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2025,10 +2032,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2064,7 +2071,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2075,13 +2082,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2160,36 +2167,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2202,7 +2209,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2264,7 +2271,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -2276,7 +2283,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>55</v>
@@ -2287,7 +2294,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -2299,13 +2306,13 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
         <v>96</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2476,7 +2483,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -2485,7 +2492,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>55</v>
@@ -2493,7 +2500,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -2502,10 +2509,10 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2580,7 +2587,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -2595,13 +2602,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
@@ -2618,7 +2625,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2683,7 +2690,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -2700,19 +2707,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +2794,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -2819,19 +2826,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>109</v>
-      </c>
-      <c r="E3" t="s">
-        <v>110</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2926,7 +2933,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -2956,16 +2963,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
         <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2995,7 +3002,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3060,7 +3067,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -3072,7 +3079,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>55</v>
@@ -3080,7 +3087,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3092,10 +3099,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3104,16 +3111,21 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6430041-C225-8845-94AF-4B32C714D3F1}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3173,7 +3185,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>204</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -3185,7 +3197,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>55</v>
@@ -3193,7 +3205,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3205,10 +3217,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3217,11 +3229,125 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3288,7 +3414,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -3300,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>55</v>
@@ -3308,7 +3434,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3320,10 +3446,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3331,7 +3457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -3404,7 +3530,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -3416,7 +3542,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>56</v>
@@ -3427,7 +3553,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -3439,149 +3565,14 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+        <v>198</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3636,10 +3627,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
         <v>169</v>
-      </c>
-      <c r="C3" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3648,10 +3639,145 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B14EC0E-8AC4-6540-9E36-1E324072B8AC}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3719,7 +3845,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3731,7 +3857,7 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -3748,19 +3874,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3782,7 +3908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -3849,7 +3975,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -3861,16 +3987,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3887,28 +4013,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3929,7 +4055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -3996,7 +4122,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4008,16 +4134,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4034,28 +4160,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4076,7 +4202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4146,7 +4272,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4158,16 +4284,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4184,28 +4310,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4226,12 +4352,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4302,7 +4428,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4314,24 +4440,24 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
@@ -4340,7 +4466,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4352,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4423,7 +4549,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4453,7 +4579,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4462,7 +4588,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4487,7 +4613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4554,7 +4680,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4566,16 +4692,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4592,7 +4718,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4601,19 +4727,19 @@
         <v>29</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4634,7 +4760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -4701,7 +4827,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -4713,16 +4839,16 @@
         <v>51</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4739,28 +4865,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="E3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4781,7 +4907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -4851,7 +4977,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -4863,10 +4989,10 @@
         <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4885,153 +5011,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
-  <dimension ref="A1:T3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-    </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -5112,7 +5107,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>44</v>
@@ -5140,10 +5135,10 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>47</v>
@@ -5165,6 +5160,137 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -5238,7 +5364,7 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -5250,7 +5376,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5269,7 +5395,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5281,7 +5407,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5292,12 +5418,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5363,7 +5489,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
@@ -5380,19 +5506,19 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -5514,7 +5640,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -5811,22 +5937,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>185</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>186</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>187</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>188</v>
-      </c>
-      <c r="I3" t="s">
-        <v>189</v>
       </c>
       <c r="J3" t="s">
         <v>30</v>
@@ -5926,7 +6052,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -5944,7 +6070,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -5962,7 +6088,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -5971,16 +6097,16 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>193</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>194</v>
-      </c>
-      <c r="G3" t="s">
-        <v>195</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6071,7 +6197,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -6089,13 +6215,13 @@
         <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6111,7 +6237,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -6120,22 +6246,22 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" t="s">
         <v>179</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>180</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>181</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>182</v>
-      </c>
-      <c r="I3" t="s">
-        <v>183</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
pushing the changes of Sanity
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC69ABCB-707C-284E-89E1-49C4CA53EE91}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC69ABCB-707C-284E-89E1-49C4CA53EE91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="22" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="30" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -26,41 +26,47 @@
     <sheet name="RS_11859" sheetId="33" r:id="rId11"/>
     <sheet name="RS_10587" sheetId="27" r:id="rId12"/>
     <sheet name="RS_10585" sheetId="26" r:id="rId13"/>
-    <sheet name="RS_10532" sheetId="25" r:id="rId14"/>
-    <sheet name="RS_10539" sheetId="24" r:id="rId15"/>
-    <sheet name="RS_10536" sheetId="34" r:id="rId16"/>
-    <sheet name="RS_10531" sheetId="35" r:id="rId17"/>
-    <sheet name="RS_10538" sheetId="23" r:id="rId18"/>
-    <sheet name="RS_10586" sheetId="22" r:id="rId19"/>
-    <sheet name="RS_10566" sheetId="21" r:id="rId20"/>
-    <sheet name="RS_10550" sheetId="20" r:id="rId21"/>
-    <sheet name="RS_10544" sheetId="19" r:id="rId22"/>
-    <sheet name="RS_10556" sheetId="18" r:id="rId23"/>
-    <sheet name="RS_10557" sheetId="17" r:id="rId24"/>
-    <sheet name="RS_10580" sheetId="16" r:id="rId25"/>
-    <sheet name="RS_10584" sheetId="43" r:id="rId26"/>
-    <sheet name="RS_10579" sheetId="14" r:id="rId27"/>
-    <sheet name="RS_10578" sheetId="13" r:id="rId28"/>
-    <sheet name="RS_10577" sheetId="12" r:id="rId29"/>
-    <sheet name="RS_10554" sheetId="11" r:id="rId30"/>
-    <sheet name="RS_10548" sheetId="44" r:id="rId31"/>
-    <sheet name="RS_10543" sheetId="42" r:id="rId32"/>
-    <sheet name="RS_10542" sheetId="10" r:id="rId33"/>
-    <sheet name="RS_10541" sheetId="9" r:id="rId34"/>
-    <sheet name="RS_10540" sheetId="8" r:id="rId35"/>
-    <sheet name="RS_10571" sheetId="36" r:id="rId36"/>
-    <sheet name="RS_10562" sheetId="37" r:id="rId37"/>
-    <sheet name="RS_10552" sheetId="7" r:id="rId38"/>
-    <sheet name="SANITY6" sheetId="6" r:id="rId39"/>
-    <sheet name="SANITY5" sheetId="5" r:id="rId40"/>
-    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId41"/>
-    <sheet name="RS_2389" sheetId="2" r:id="rId42"/>
-    <sheet name="RS_10569" sheetId="15" r:id="rId43"/>
+    <sheet name="RS_11179" sheetId="45" r:id="rId14"/>
+    <sheet name="RS_10532" sheetId="25" r:id="rId15"/>
+    <sheet name="RS_10539" sheetId="24" r:id="rId16"/>
+    <sheet name="RS_10536" sheetId="34" r:id="rId17"/>
+    <sheet name="RS_10531" sheetId="35" r:id="rId18"/>
+    <sheet name="RS_10538" sheetId="23" r:id="rId19"/>
+    <sheet name="RS_10586" sheetId="22" r:id="rId20"/>
+    <sheet name="RS_10566" sheetId="21" r:id="rId21"/>
+    <sheet name="RS_10550" sheetId="20" r:id="rId22"/>
+    <sheet name="RS_10544" sheetId="19" r:id="rId23"/>
+    <sheet name="RS_10556" sheetId="18" r:id="rId24"/>
+    <sheet name="RS_10557" sheetId="17" r:id="rId25"/>
+    <sheet name="RS_10580" sheetId="16" r:id="rId26"/>
+    <sheet name="RS_10584" sheetId="43" r:id="rId27"/>
+    <sheet name="RS_10579" sheetId="14" r:id="rId28"/>
+    <sheet name="RS_10578" sheetId="13" r:id="rId29"/>
+    <sheet name="RS_10577" sheetId="12" r:id="rId30"/>
+    <sheet name="RS_10554" sheetId="11" r:id="rId31"/>
+    <sheet name="RS_10548" sheetId="44" r:id="rId32"/>
+    <sheet name="RS_10543" sheetId="42" r:id="rId33"/>
+    <sheet name="RS_10542" sheetId="10" r:id="rId34"/>
+    <sheet name="RS_10541" sheetId="9" r:id="rId35"/>
+    <sheet name="RS_10540" sheetId="8" r:id="rId36"/>
+    <sheet name="RS_10571" sheetId="36" r:id="rId37"/>
+    <sheet name="RS_10562" sheetId="37" r:id="rId38"/>
+    <sheet name="RS_10552" sheetId="7" r:id="rId39"/>
+    <sheet name="SANITY6" sheetId="6" r:id="rId40"/>
+    <sheet name="SANITY5" sheetId="5" r:id="rId41"/>
+    <sheet name="Scenario7_Checklist" sheetId="4" r:id="rId42"/>
+    <sheet name="RS_2389" sheetId="2" r:id="rId43"/>
+    <sheet name="RS_10569" sheetId="15" r:id="rId44"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -70,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="214">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -141,6 +147,27 @@
     <t>Product Name</t>
   </si>
   <si>
+    <t>WO-00003658</t>
+  </si>
+  <si>
+    <t>P105332610201816037</t>
+  </si>
+  <si>
+    <t>RS_10514_Calender_4</t>
+  </si>
+  <si>
+    <t>TechName2</t>
+  </si>
+  <si>
+    <t>Salesforceuser</t>
+  </si>
+  <si>
+    <t>Auto_Tech_Service_user1</t>
+  </si>
+  <si>
+    <t>0050t000001PqX7AAK</t>
+  </si>
+  <si>
     <t>RS_10525_Calender_6</t>
   </si>
   <si>
@@ -162,6 +189,9 @@
     <t>Work Orders</t>
   </si>
   <si>
+    <t>WO-00004336</t>
+  </si>
+  <si>
     <t>a240t000000GglLAAS</t>
   </si>
   <si>
@@ -204,24 +234,90 @@
     <t>TechName1</t>
   </si>
   <si>
-    <t>TechName2</t>
-  </si>
-  <si>
-    <t>Salesforceuser</t>
+    <t>WO-00004300</t>
+  </si>
+  <si>
+    <t>WO-00004301</t>
+  </si>
+  <si>
+    <t>WO-00004302</t>
+  </si>
+  <si>
+    <t>WO-00004303</t>
+  </si>
+  <si>
+    <t>WO-00004304</t>
+  </si>
+  <si>
+    <t>WO-00004305</t>
   </si>
   <si>
     <t>a240t000000L5IxAAK</t>
   </si>
   <si>
-    <t>0050t000001PqX7AAK</t>
+    <t>RS_10512_Calender_2</t>
+  </si>
+  <si>
+    <t>WO_SVMX_4</t>
+  </si>
+  <si>
+    <t>WO-00004313</t>
+  </si>
+  <si>
+    <t>WO-00004314</t>
+  </si>
+  <si>
+    <t>WO-00004315</t>
+  </si>
+  <si>
+    <t>WO-00004316</t>
+  </si>
+  <si>
+    <t>RS_10515_Calender_5</t>
+  </si>
+  <si>
+    <t>WO_SVMX_5</t>
+  </si>
+  <si>
+    <t>WO_SVMX_6</t>
+  </si>
+  <si>
+    <t>WO-00004121</t>
+  </si>
+  <si>
+    <t>WO-00004122</t>
+  </si>
+  <si>
+    <t>WO-00004123</t>
+  </si>
+  <si>
+    <t>WO-00004124</t>
+  </si>
+  <si>
+    <t>WO-00004125</t>
+  </si>
+  <si>
+    <t>WO-00004126</t>
   </si>
   <si>
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
+    <t>WO-00004367</t>
+  </si>
+  <si>
+    <t>WO-00004368</t>
+  </si>
+  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
+    <t>WO-00004310</t>
+  </si>
+  <si>
+    <t>WO-00004311</t>
+  </si>
+  <si>
     <t>SCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
@@ -258,6 +354,9 @@
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
   </si>
   <si>
+    <t>AUTO_EDIT_WORKORDER</t>
+  </si>
+  <si>
     <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
@@ -276,6 +375,18 @@
     <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
   </si>
   <si>
+    <t>SCN_RS_11179</t>
+  </si>
+  <si>
+    <t>Service Report Name</t>
+  </si>
+  <si>
+    <t>RS_11179</t>
+  </si>
+  <si>
+    <t>Work Order Service Report</t>
+  </si>
+  <si>
     <t>SCN_GetPriceNotCovered_RS_10532</t>
   </si>
   <si>
@@ -300,6 +411,21 @@
     <t>Installed Product Name</t>
   </si>
   <si>
+    <t>WO-00000002</t>
+  </si>
+  <si>
+    <t>P1053915112018111331</t>
+  </si>
+  <si>
+    <t>P1053915112018111332</t>
+  </si>
+  <si>
+    <t>AutoScon1511201811620</t>
+  </si>
+  <si>
+    <t>Auto_10539151120181167</t>
+  </si>
+  <si>
     <t>IB1053918102018142834</t>
   </si>
   <si>
@@ -405,6 +531,15 @@
     <t>ManualSCN_Checklist_4_RS-10580_Checklist_Sections</t>
   </si>
   <si>
+    <t>SCN_ChecklistAttachment_RS-10584</t>
+  </si>
+  <si>
+    <t>Data_SCN_ChecklistAttachment_RS_10584</t>
+  </si>
+  <si>
+    <t>SCN_Checklist_Attachment</t>
+  </si>
+  <si>
     <t>SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
   </si>
   <si>
@@ -420,6 +555,9 @@
     <t>Data_SCN_Checklist_2_RS-10578_DVR</t>
   </si>
   <si>
+    <t>Auto_10578_ChecklistDVR</t>
+  </si>
+  <si>
     <t>SCN_Checklist_1_RS-10577_SOU</t>
   </si>
   <si>
@@ -435,6 +573,33 @@
     <t>RS_10554_field_mapping</t>
   </si>
   <si>
+    <t>RS_10548</t>
+  </si>
+  <si>
+    <t>SCN_RS_10548</t>
+  </si>
+  <si>
+    <t>RS_10548 Multi Field WO Search</t>
+  </si>
+  <si>
+    <t>RS_10543</t>
+  </si>
+  <si>
+    <t>BillingType</t>
+  </si>
+  <si>
+    <t>SCN_RS_10543</t>
+  </si>
+  <si>
+    <t>RS_10543 SFM Search for Multi Page View</t>
+  </si>
+  <si>
+    <t>SanityScenario5</t>
+  </si>
+  <si>
+    <t>Empowerment</t>
+  </si>
+  <si>
     <t>RS_10542</t>
   </si>
   <si>
@@ -444,9 +609,6 @@
     <t>OrderStatus</t>
   </si>
   <si>
-    <t>BillingType</t>
-  </si>
-  <si>
     <t>ProductName1</t>
   </si>
   <si>
@@ -534,9 +696,6 @@
     <t>DATA_SANITY5</t>
   </si>
   <si>
-    <t>SanityScenario5</t>
-  </si>
-  <si>
     <t>Rule is billing type cannot be loan</t>
   </si>
   <si>
@@ -559,154 +718,13 @@
   </si>
   <si>
     <t>DATA_SCN_ScheduledDataSync_RS_10569</t>
-  </si>
-  <si>
-    <t>WO-00003658</t>
-  </si>
-  <si>
-    <t>P105332610201816037</t>
-  </si>
-  <si>
-    <t>Auto_Tech_Service_user1</t>
-  </si>
-  <si>
-    <t>RS_10514_Calender_4</t>
-  </si>
-  <si>
-    <t>RS_10512_Calender_2</t>
-  </si>
-  <si>
-    <t>WO_SVMX_4</t>
-  </si>
-  <si>
-    <t>RS_10515_Calender_5</t>
-  </si>
-  <si>
-    <t>WO_SVMX_5</t>
-  </si>
-  <si>
-    <t>WO_SVMX_6</t>
-  </si>
-  <si>
-    <t>WO-00004121</t>
-  </si>
-  <si>
-    <t>WO-00004122</t>
-  </si>
-  <si>
-    <t>WO-00004123</t>
-  </si>
-  <si>
-    <t>WO-00004124</t>
-  </si>
-  <si>
-    <t>WO-00004125</t>
-  </si>
-  <si>
-    <t>WO-00004126</t>
-  </si>
-  <si>
-    <t>WO-00004300</t>
-  </si>
-  <si>
-    <t>WO-00004301</t>
-  </si>
-  <si>
-    <t>WO-00004302</t>
-  </si>
-  <si>
-    <t>WO-00004303</t>
-  </si>
-  <si>
-    <t>WO-00004304</t>
-  </si>
-  <si>
-    <t>WO-00004305</t>
-  </si>
-  <si>
-    <t>WO-00004310</t>
-  </si>
-  <si>
-    <t>WO-00004311</t>
-  </si>
-  <si>
-    <t>WO-00004313</t>
-  </si>
-  <si>
-    <t>WO-00004314</t>
-  </si>
-  <si>
-    <t>WO-00004315</t>
-  </si>
-  <si>
-    <t>WO-00004316</t>
-  </si>
-  <si>
-    <t>WO-00004336</t>
-  </si>
-  <si>
-    <t>WO-00004367</t>
-  </si>
-  <si>
-    <t>WO-00004368</t>
-  </si>
-  <si>
-    <t>AUTO_EDIT_WORKORDER</t>
-  </si>
-  <si>
-    <t>Auto_10578_ChecklistDVR</t>
-  </si>
-  <si>
-    <t>RS_10543</t>
-  </si>
-  <si>
-    <t>SCN_RS_10543</t>
-  </si>
-  <si>
-    <t>RS_10543 SFM Search for Multi Page View</t>
-  </si>
-  <si>
-    <t>Empowerment</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistAttachment_RS-10584</t>
-  </si>
-  <si>
-    <t>Data_SCN_ChecklistAttachment_RS_10584</t>
-  </si>
-  <si>
-    <t>SCN_Checklist_Attachment</t>
-  </si>
-  <si>
-    <t>WO-00000002</t>
-  </si>
-  <si>
-    <t>P1053915112018111331</t>
-  </si>
-  <si>
-    <t>P1053915112018111332</t>
-  </si>
-  <si>
-    <t>AutoScon1511201811620</t>
-  </si>
-  <si>
-    <t>Auto_10539151120181167</t>
-  </si>
-  <si>
-    <t>RS_10548 Multi Field WO Search</t>
-  </si>
-  <si>
-    <t>RS_10548</t>
-  </si>
-  <si>
-    <t>SCN_RS_10548</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -882,10 +900,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1201,24 +1219,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1291,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1300,7 @@
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1301,17 +1319,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,21 +1384,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1398,21 +1416,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>75</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>192</v>
+        <v>76</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1434,16 +1452,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="42" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1498,21 +1517,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1530,21 +1549,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>79</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1566,13 +1585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FF0BDA26-1AD6-5648-BD9A-E01AA4DDCA7C}"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1627,62 +1644,62 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1694,13 +1711,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C67EF94B-0B3B-5838-830C-E3A509766221}">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1755,50 +1772,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1807,84 +1824,41 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCA38FB-8D8A-490E-A047-17088434D768}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{9F0B533A-B770-5033-BEB3-A3D5E1E7BAA9}">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1893,20 +1867,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0" xr3:uid="{274F5AE0-5452-572F-8038-C13FFDA59D49}">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1961,50 +1931,20 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G3" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2013,41 +1953,118 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{33642244-9AC9-5136-AF77-195C889548CE}">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2056,51 +2073,41 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D624DF06-3800-545C-AC8D-BADC89115800}">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="16" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2109,20 +2116,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{11A3ACCB-1F19-5AC9-A611-4158731A345D}">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2132,83 +2140,27 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2217,16 +2169,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2281,50 +2237,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>122</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2336,13 +2280,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2341,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2408,7 +2352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2425,20 +2369,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2493,38 +2433,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>92</v>
+      <c r="G3" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2533,16 +2485,20 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2597,35 +2553,39 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8"/>
+        <v>134</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2633,19 +2593,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2700,39 +2657,35 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>193</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2740,16 +2693,123 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2804,21 +2864,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -2836,21 +2896,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2874,21 +2934,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2943,18 +3003,18 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2973,18 +3033,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3009,20 +3069,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3077,162 +3137,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6430041-C225-8845-94AF-4B32C714D3F1}">
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3241,20 +3183,24 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6430041-C225-8845-94AF-4B32C714D3F1}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0" xr3:uid="{2E8AB339-ED93-55BB-8E39-0ACA3CF81A91}">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3309,44 +3255,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3355,21 +3301,20 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3424,44 +3369,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3470,22 +3415,21 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3540,50 +3484,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3595,18 +3533,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -3634,15 +3572,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3651,21 +3589,143 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{EE242A16-C6B8-5192-B120-522BC795EE76}">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3720,18 +3780,18 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3750,18 +3810,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3785,23 +3845,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE1A733-210B-6A4C-914A-7488D3B97413}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{E5803408-9CEB-5998-AE20-ED21441223B1}">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3856,12 +3916,12 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -3879,12 +3939,12 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3909,22 +3969,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B14EC0E-8AC4-6540-9E36-1E324072B8AC}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FB51155B-C3EB-5C85-9567-9E582AE8EA05}">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3979,21 +4039,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4008,21 +4068,21 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -4044,17 +4104,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7075697D-051A-5480-9A35-AA80E904E1A1}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4109,30 +4169,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4147,30 +4207,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4191,17 +4251,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C7A11F4D-6E51-5B1A-9CF2-8FFD2B06F078}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4256,30 +4316,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4294,30 +4354,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>133</v>
+        <v>185</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4338,20 +4398,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D979DC6D-665A-5B40-B235-9A07D260EAB6}">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4406,30 +4466,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4444,30 +4504,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4488,26 +4548,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CAA03FB3-9A95-5D50-9E3C-B000AFB1AE50}">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4562,47 +4622,47 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="9">
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4614,21 +4674,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{62E455AB-44C1-5DAA-A80F-CFF2989D01C0}">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4683,18 +4743,18 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -4713,18 +4773,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4749,17 +4809,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{E6B2BAC2-667D-5CCD-8069-8C8F7D962337}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4814,30 +4874,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>145</v>
+        <v>197</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4852,30 +4912,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4896,170 +4956,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5114,15 +5027,15 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -5142,15 +5055,15 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E3" s="17"/>
       <c r="M3" s="8"/>
@@ -5169,19 +5082,166 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{BF3E6036-5CFF-541C-9DD1-8B260238869F}">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1"/>
+      <c r="S1"/>
+    </row>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44C9DB06-433C-50F5-8210-7EB2F2901AA3}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5236,24 +5296,24 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5270,24 +5330,24 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5295,24 +5355,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{8CA7FA36-F026-53D8-85D7-7434F22EA588}">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5367,24 +5427,24 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5401,24 +5461,24 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -5426,24 +5486,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{87752282-9950-53E0-ACC6-858909551C9B}">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5498,21 +5558,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5529,21 +5589,21 @@
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5554,24 +5614,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FB84E6B5-2F03-524A-B55D-05F6A9FA1888}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5623,38 +5683,38 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="8" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5666,19 +5726,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5733,21 +5793,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -5765,21 +5825,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>190</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -5806,20 +5866,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5874,21 +5934,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -5906,21 +5966,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -5947,21 +6007,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6016,42 +6076,42 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
@@ -6062,42 +6122,42 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6118,20 +6178,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6186,27 +6246,27 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -6222,27 +6282,27 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6263,20 +6323,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6331,33 +6391,33 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6371,33 +6431,33 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>173</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>174</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>175</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>176</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
updating testdata as there is name mismatch in sahi file and appium side
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC69ABCB-707C-284E-89E1-49C4CA53EE91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E79D2E-6D0F-B149-986B-7562635D579B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="30" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="29" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -58,15 +58,10 @@
     <sheet name="RS_2389" sheetId="2" r:id="rId43"/>
     <sheet name="RS_10569" sheetId="15" r:id="rId44"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -76,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="215">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -705,26 +700,29 @@
     <t>Data_Scenario7_Checklist</t>
   </si>
   <si>
-    <t>Scenario7_checklist</t>
-  </si>
-  <si>
     <t>RS_2389_checklist</t>
   </si>
   <si>
-    <t>SFM_Auto_2372018162541</t>
-  </si>
-  <si>
     <t>SCN_ScheduledDataSync_RS_10569</t>
   </si>
   <si>
     <t>DATA_SCN_ScheduledDataSync_RS_10569</t>
+  </si>
+  <si>
+    <t>Sanity2_Checklist</t>
+  </si>
+  <si>
+    <t>Sanity7_checklist</t>
+  </si>
+  <si>
+    <t>Checklist_OPDOC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +789,12 @@
       <sz val="11"/>
       <color rgb="FF3933FF"/>
       <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -870,7 +874,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -898,6 +902,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1219,24 +1224,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1296,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1305,7 @@
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1319,17 +1324,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1389,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>74</v>
       </c>
@@ -1416,7 +1421,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1452,17 +1457,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1522,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>77</v>
       </c>
@@ -1549,7 +1554,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1585,11 +1590,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FF0BDA26-1AD6-5648-BD9A-E01AA4DDCA7C}"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1644,7 +1649,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1673,7 +1678,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>87</v>
       </c>
@@ -1711,13 +1716,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C67EF94B-0B3B-5838-830C-E3A509766221}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1777,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>94</v>
       </c>
@@ -1795,7 +1800,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>96</v>
       </c>
@@ -1827,17 +1832,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCA38FB-8D8A-490E-A047-17088434D768}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{9F0B533A-B770-5033-BEB3-A3D5E1E7BAA9}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1853,7 +1858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1870,13 +1875,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0" xr3:uid="{274F5AE0-5452-572F-8038-C13FFDA59D49}">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1936,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>103</v>
       </c>
@@ -1939,7 +1944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -1956,17 +1961,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{33642244-9AC9-5136-AF77-195C889548CE}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2026,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>105</v>
       </c>
@@ -2044,7 +2049,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -2076,17 +2081,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D624DF06-3800-545C-AC8D-BADC89115800}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>117</v>
       </c>
@@ -2102,7 +2107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2119,18 +2124,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{11A3ACCB-1F19-5AC9-A611-4158731A345D}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2141,7 +2146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>119</v>
       </c>
@@ -2152,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -2172,17 +2177,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2242,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>122</v>
       </c>
@@ -2254,7 +2259,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -2280,13 +2285,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2341,7 +2346,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2372,13 +2377,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +2438,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>128</v>
       </c>
@@ -2456,7 +2461,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>129</v>
       </c>
@@ -2488,17 +2493,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2553,7 +2558,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>132</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>132</v>
       </c>
@@ -2596,13 +2601,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2657,7 +2662,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>135</v>
       </c>
@@ -2672,7 +2677,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>136</v>
       </c>
@@ -2696,16 +2701,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2760,7 +2765,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>138</v>
       </c>
@@ -2777,7 +2782,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>139</v>
       </c>
@@ -2803,13 +2808,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2864,7 +2869,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>141</v>
       </c>
@@ -2896,7 +2901,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2938,17 +2943,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3003,7 +3008,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>145</v>
       </c>
@@ -3033,7 +3038,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -3073,16 +3078,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3137,7 +3142,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>148</v>
       </c>
@@ -3157,7 +3162,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>149</v>
       </c>
@@ -3186,21 +3191,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6430041-C225-8845-94AF-4B32C714D3F1}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{2E8AB339-ED93-55BB-8E39-0ACA3CF81A91}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3255,7 +3260,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>151</v>
       </c>
@@ -3275,7 +3280,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>152</v>
       </c>
@@ -3304,17 +3309,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3374,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>154</v>
       </c>
@@ -3389,7 +3394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>155</v>
       </c>
@@ -3418,18 +3423,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3484,7 +3489,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>157</v>
       </c>
@@ -3504,7 +3509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>158</v>
       </c>
@@ -3533,18 +3538,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3561,7 +3566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -3572,7 +3577,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3592,19 +3597,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3664,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>160</v>
       </c>
@@ -3682,7 +3687,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>161</v>
       </c>
@@ -3714,18 +3719,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{EE242A16-C6B8-5192-B120-522BC795EE76}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3780,7 +3785,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>163</v>
       </c>
@@ -3810,7 +3815,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -3849,19 +3854,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE1A733-210B-6A4C-914A-7488D3B97413}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{E5803408-9CEB-5998-AE20-ED21441223B1}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3916,7 +3921,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>165</v>
       </c>
@@ -3939,7 +3944,7 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>166</v>
       </c>
@@ -3973,18 +3978,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B14EC0E-8AC4-6540-9E36-1E324072B8AC}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FB51155B-C3EB-5C85-9567-9E582AE8EA05}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4039,7 +4044,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>168</v>
       </c>
@@ -4068,7 +4073,7 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>170</v>
       </c>
@@ -4108,13 +4113,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7075697D-051A-5480-9A35-AA80E904E1A1}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4169,7 +4174,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>174</v>
       </c>
@@ -4207,7 +4212,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>178</v>
       </c>
@@ -4255,13 +4260,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C7A11F4D-6E51-5B1A-9CF2-8FFD2B06F078}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4316,7 +4321,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>184</v>
       </c>
@@ -4354,7 +4359,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>185</v>
       </c>
@@ -4402,16 +4407,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D979DC6D-665A-5B40-B235-9A07D260EAB6}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4466,7 +4471,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>186</v>
       </c>
@@ -4504,7 +4509,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>187</v>
       </c>
@@ -4552,22 +4557,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CAA03FB3-9A95-5D50-9E3C-B000AFB1AE50}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4622,7 +4627,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>188</v>
       </c>
@@ -4645,7 +4650,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>192</v>
       </c>
@@ -4678,17 +4683,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{62E455AB-44C1-5DAA-A80F-CFF2989D01C0}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4743,7 +4748,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>194</v>
       </c>
@@ -4773,7 +4778,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>195</v>
       </c>
@@ -4813,13 +4818,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{E6B2BAC2-667D-5CCD-8069-8C8F7D962337}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4874,7 +4879,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
@@ -4912,7 +4917,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>198</v>
       </c>
@@ -4960,19 +4965,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5027,7 +5032,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -5055,7 +5060,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -5085,13 +5090,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{BF3E6036-5CFF-541C-9DD1-8B260238869F}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5146,7 +5151,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>200</v>
       </c>
@@ -5184,7 +5189,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>201</v>
       </c>
@@ -5232,16 +5237,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44C9DB06-433C-50F5-8210-7EB2F2901AA3}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5296,7 +5301,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>204</v>
       </c>
@@ -5330,7 +5335,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>205</v>
       </c>
@@ -5359,20 +5364,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{8CA7FA36-F026-53D8-85D7-7434F22EA588}">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5427,7 +5432,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -5461,7 +5466,7 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>208</v>
       </c>
@@ -5475,10 +5480,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5490,20 +5495,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{87752282-9950-53E0-ACC6-858909551C9B}">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5558,9 +5563,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5589,9 +5594,9 @@
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5602,8 +5607,8 @@
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>211</v>
+      <c r="E3" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5618,20 +5623,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FB84E6B5-2F03-524A-B55D-05F6A9FA1888}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5683,9 +5688,9 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5700,9 +5705,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5726,19 +5731,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5793,7 +5798,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -5825,7 +5830,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -5866,20 +5871,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5934,7 +5939,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>39</v>
       </c>
@@ -5966,7 +5971,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -6007,21 +6012,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6076,7 +6081,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
@@ -6122,7 +6127,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -6178,20 +6183,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6246,7 +6251,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>59</v>
       </c>
@@ -6282,7 +6287,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -6323,20 +6328,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6391,7 +6396,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>65</v>
       </c>
@@ -6431,7 +6436,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
updated checklist process names
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{41CD3FE7-D555-1649-B81A-7F80CBFFF001}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7172F0-F69C-C644-9290-5BBCDD20FFE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="29" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -365,12 +365,6 @@
     <t>Data_SCN_ChecklistOPDOC_1_RS-10585</t>
   </si>
   <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10585_inProg</t>
-  </si>
-  <si>
-    <t>Manual_RS10585_ChecklistOPDOC_InProgOP</t>
-  </si>
-  <si>
     <t>SCN_RS_11179</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
   </si>
   <si>
-    <t>ManualSCN_Checklist_4_RS-10580_Checklist_Sections</t>
-  </si>
-  <si>
     <t>SCN_ChecklistAttachment_RS-10584</t>
   </si>
   <si>
@@ -542,9 +533,6 @@
     <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
   </si>
   <si>
-    <t>ManualSCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
-  </si>
-  <si>
     <t>SCN_Checklist_2_RS-10578_DVR</t>
   </si>
   <si>
@@ -726,6 +714,18 @@
   </si>
   <si>
     <t>RS_10549 Multi Field WO Search</t>
+  </si>
+  <si>
+    <t>Auto_10585_ChecklistOPDOC</t>
+  </si>
+  <si>
+    <t>Auto_RS10585_ChecklistOPDOC_InProgOP</t>
+  </si>
+  <si>
+    <t>Auto_10579_Checklist</t>
+  </si>
+  <si>
+    <t>Auto_10580_ChecklistSections</t>
   </si>
 </sst>
 </file>
@@ -1726,11 +1726,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1824,13 +1830,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1862,18 +1868,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1948,7 +1954,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1956,10 +1962,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2038,48 +2044,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>112</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>113</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>114</v>
-      </c>
-      <c r="F3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2111,7 +2117,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2119,10 +2125,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2158,7 +2164,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2169,13 +2175,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2254,36 +2260,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>125</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2450,7 +2456,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2473,7 +2479,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2485,13 +2491,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2570,7 +2576,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2579,7 +2585,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>85</v>
@@ -2587,7 +2593,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2596,10 +2602,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2674,7 +2680,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2689,13 +2695,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2777,7 +2783,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2794,13 +2800,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2881,7 +2887,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2913,19 +2919,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
         <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>144</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3020,7 +3026,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3050,16 +3056,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3089,12 +3095,13 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3154,7 +3161,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3174,7 +3181,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3186,7 +3193,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
@@ -3272,7 +3279,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3292,7 +3299,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3304,7 +3311,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
@@ -3320,12 +3327,13 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -3386,7 +3394,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3406,7 +3414,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3418,7 +3426,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
@@ -3434,7 +3442,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3501,7 +3509,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3521,7 +3529,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3533,7 +3541,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>92</v>
@@ -3608,7 +3616,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3676,7 +3684,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3699,7 +3707,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3711,10 +3719,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>92</v>
@@ -3797,7 +3805,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3827,16 +3835,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3933,7 +3941,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3956,10 +3964,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4057,7 +4065,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4080,10 +4088,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4180,7 +4188,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4192,7 +4200,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4209,19 +4217,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -4310,7 +4318,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4322,16 +4330,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4348,28 +4356,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4457,7 +4465,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4469,16 +4477,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4495,28 +4503,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4607,7 +4615,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4619,16 +4627,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4645,28 +4653,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4763,7 +4771,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4775,18 +4783,18 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4801,7 +4809,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4884,7 +4892,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4914,7 +4922,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4923,7 +4931,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -5140,7 +5148,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5152,16 +5160,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5178,7 +5186,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5187,19 +5195,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5290,7 +5298,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5302,16 +5310,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5328,28 +5336,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5375,7 +5383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -5441,7 +5449,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5453,10 +5461,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5475,22 +5483,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5572,7 +5580,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5606,7 +5614,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5618,10 +5626,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5703,7 +5711,7 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5734,7 +5742,7 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5746,7 +5754,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5828,7 +5836,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5845,7 +5853,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
added retry analyser cleaned up scripts
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7172F0-F69C-C644-9290-5BBCDD20FFE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844823E6-568C-E948-9D45-A312E91E608D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -341,21 +341,9 @@
     <t>Default title for Checklist</t>
   </si>
   <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_allversions</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
-  </si>
-  <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
-  </si>
-  <si>
     <t>AUTO_EDIT_WORKORDER</t>
   </si>
   <si>
-    <t>ManualSCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
     <t>SCN_ChecklistOPDOC_1_RS-10585</t>
   </si>
   <si>
@@ -458,12 +446,6 @@
     <t>Data_SCN_ChecklistOPDOC_2_RS-10586</t>
   </si>
   <si>
-    <t>ManualSCN_ChecklistOPDOC_2_RS-10586snd</t>
-  </si>
-  <si>
-    <t>Manual_RS10586_ChecklistOPDOC</t>
-  </si>
-  <si>
     <t>RS_10566_Acc_Pro_History</t>
   </si>
   <si>
@@ -726,6 +708,24 @@
   </si>
   <si>
     <t>Auto_10580_ChecklistSections</t>
+  </si>
+  <si>
+    <t>Auto_10586_ChecklistOPDOC_DynamicRes</t>
+  </si>
+  <si>
+    <t>OPDOC_10586_ChecklistOPDOC_DynamicRes</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_allversions</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
+  </si>
+  <si>
+    <t>Auto_SCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
 </sst>
 </file>
@@ -1600,9 +1600,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1702,19 +1711,19 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1726,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1795,7 +1804,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1807,7 +1816,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -1818,7 +1827,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -1830,13 +1839,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1868,18 +1877,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1963,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1962,10 +1971,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2044,48 +2053,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2117,7 +2126,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2125,10 +2134,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2164,7 +2173,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2175,13 +2184,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2260,36 +2269,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
         <v>120</v>
       </c>
-      <c r="B3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2394,10 +2403,15 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2456,7 +2470,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2468,7 +2482,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -2479,7 +2493,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2490,14 +2504,14 @@
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
-        <v>128</v>
+      <c r="E3" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2576,7 +2590,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2585,7 +2599,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>85</v>
@@ -2593,7 +2607,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2602,10 +2616,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2680,7 +2694,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2695,13 +2709,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2783,7 +2797,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2800,19 +2814,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2887,7 +2901,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2919,19 +2933,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3026,7 +3040,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3056,16 +3070,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3161,7 +3175,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3173,7 +3187,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -3181,7 +3195,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3193,10 +3207,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3279,7 +3293,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3291,7 +3305,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -3299,7 +3313,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3311,10 +3325,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3394,7 +3408,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3406,7 +3420,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -3414,7 +3428,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3426,10 +3440,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3509,7 +3523,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3521,7 +3535,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>85</v>
@@ -3529,7 +3543,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3541,10 +3555,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3684,7 +3698,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3696,7 +3710,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>86</v>
@@ -3707,7 +3721,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3719,13 +3733,13 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3805,7 +3819,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3835,16 +3849,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3941,7 +3955,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3964,10 +3978,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4065,7 +4079,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4088,10 +4102,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4188,7 +4202,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4200,7 +4214,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4217,19 +4231,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -4318,7 +4332,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4330,16 +4344,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4356,28 +4370,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4465,7 +4479,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4477,16 +4491,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4503,28 +4517,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4615,7 +4629,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4627,16 +4641,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4653,28 +4667,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4771,7 +4785,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4783,24 +4797,24 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -4809,7 +4823,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4892,7 +4906,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4922,7 +4936,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4931,7 +4945,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -5148,7 +5162,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5160,16 +5174,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5186,7 +5200,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5195,19 +5209,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5298,7 +5312,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5310,16 +5324,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5336,28 +5350,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5449,7 +5463,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5461,10 +5475,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5483,22 +5497,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5580,7 +5594,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5592,7 +5606,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>86</v>
@@ -5614,7 +5628,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5626,10 +5640,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5711,7 +5725,7 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5723,7 +5737,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5742,7 +5756,7 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5754,7 +5768,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5836,7 +5850,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5853,19 +5867,19 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding tech id to config file
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B160B21-FA6E-0F4D-B29C-2A8E40A3F13F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="30" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
     <sheet name="RS_2389" sheetId="2" r:id="rId45"/>
     <sheet name="RS_10569" sheetId="15" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -186,9 +185,6 @@
     <t>Work Orders</t>
   </si>
   <si>
-    <t>WO-00004336</t>
-  </si>
-  <si>
     <t>a240t000000GglLAAS</t>
   </si>
   <si>
@@ -231,24 +227,6 @@
     <t>TechName1</t>
   </si>
   <si>
-    <t>WO-00004300</t>
-  </si>
-  <si>
-    <t>WO-00004301</t>
-  </si>
-  <si>
-    <t>WO-00004302</t>
-  </si>
-  <si>
-    <t>WO-00004303</t>
-  </si>
-  <si>
-    <t>WO-00004304</t>
-  </si>
-  <si>
-    <t>WO-00004305</t>
-  </si>
-  <si>
     <t>a240t000000L5IxAAK</t>
   </si>
   <si>
@@ -258,18 +236,6 @@
     <t>WO_SVMX_4</t>
   </si>
   <si>
-    <t>WO-00004313</t>
-  </si>
-  <si>
-    <t>WO-00004314</t>
-  </si>
-  <si>
-    <t>WO-00004315</t>
-  </si>
-  <si>
-    <t>WO-00004316</t>
-  </si>
-  <si>
     <t>RS_10515_Calender_5</t>
   </si>
   <si>
@@ -279,42 +245,12 @@
     <t>WO_SVMX_6</t>
   </si>
   <si>
-    <t>WO-00004121</t>
-  </si>
-  <si>
-    <t>WO-00004122</t>
-  </si>
-  <si>
-    <t>WO-00004123</t>
-  </si>
-  <si>
-    <t>WO-00004124</t>
-  </si>
-  <si>
-    <t>WO-00004125</t>
-  </si>
-  <si>
-    <t>WO-00004126</t>
-  </si>
-  <si>
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
-    <t>WO-00004367</t>
-  </si>
-  <si>
-    <t>WO-00004368</t>
-  </si>
-  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
-    <t>WO-00004310</t>
-  </si>
-  <si>
-    <t>WO-00004311</t>
-  </si>
-  <si>
     <t>SCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
@@ -736,12 +672,75 @@
   </si>
   <si>
     <t>RS_10545 Multi Field WO Search</t>
+  </si>
+  <si>
+    <t>WO-00005804</t>
+  </si>
+  <si>
+    <t>WO-00005805</t>
+  </si>
+  <si>
+    <t>WO-00005806</t>
+  </si>
+  <si>
+    <t>WO-00005807</t>
+  </si>
+  <si>
+    <t>WO-00005808</t>
+  </si>
+  <si>
+    <t>WO-00005809</t>
+  </si>
+  <si>
+    <t>WO-00005810</t>
+  </si>
+  <si>
+    <t>WO-00005820</t>
+  </si>
+  <si>
+    <t>WO-00005821</t>
+  </si>
+  <si>
+    <t>WO-00005826</t>
+  </si>
+  <si>
+    <t>WO-00005827</t>
+  </si>
+  <si>
+    <t>WO-00005834</t>
+  </si>
+  <si>
+    <t>WO-00005835</t>
+  </si>
+  <si>
+    <t>WO-00005836</t>
+  </si>
+  <si>
+    <t>WO-00005837</t>
+  </si>
+  <si>
+    <t>WO-00005850</t>
+  </si>
+  <si>
+    <t>WO-00005851</t>
+  </si>
+  <si>
+    <t>WO-00005852</t>
+  </si>
+  <si>
+    <t>WO-00005853</t>
+  </si>
+  <si>
+    <t>WO-00005854</t>
+  </si>
+  <si>
+    <t>WO-00005855</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1241,7 +1240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
@@ -1341,7 +1340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1411,7 +1410,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -1420,10 +1419,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1443,7 +1442,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1452,10 +1451,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1474,7 +1473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1483,7 +1482,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1544,7 +1543,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -1553,10 +1552,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1576,7 +1575,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1585,10 +1584,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>210</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1607,7 +1606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
@@ -1616,11 +1615,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="42.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="43" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1680,60 +1679,60 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="G3" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -1751,10 +1750,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1814,48 +1813,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1864,17 +1863,17 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCA38FB-8D8A-490E-A047-17088434D768}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1887,18 +1886,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +1906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
@@ -1973,7 +1972,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1981,10 +1980,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1993,7 +1992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2063,48 +2062,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2113,7 +2112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2136,7 +2135,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2144,10 +2143,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2156,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2183,7 +2182,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2194,13 +2193,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2209,7 +2208,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2279,36 +2278,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2409,7 +2408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2418,9 +2417,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2480,48 +2479,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2530,7 +2529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2600,7 +2599,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2609,15 +2608,15 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2626,10 +2625,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2638,7 +2637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2704,13 +2703,13 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
@@ -2719,13 +2718,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2738,7 +2737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2807,36 +2806,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2845,7 +2844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -2911,7 +2910,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2920,7 +2919,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>33</v>
@@ -2943,19 +2942,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2980,7 +2979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3050,7 +3049,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3059,7 +3058,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3080,16 +3079,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3115,7 +3114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3125,7 +3124,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3185,42 +3184,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3229,10 +3228,10 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6430041-C225-8845-94AF-4B32C714D3F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3303,42 +3302,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3347,7 +3346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3357,7 +3356,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -3418,42 +3417,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3462,7 +3461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3533,42 +3532,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3577,7 +3576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3636,7 +3635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3708,48 +3707,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3758,7 +3757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3829,7 +3828,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3838,7 +3837,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3859,16 +3858,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3893,7 +3892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB040C19-3CAE-FB4A-8E34-1DADD6BBCE3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3902,7 +3901,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
@@ -3965,7 +3964,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3988,10 +3987,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4017,7 +4016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE1A733-210B-6A4C-914A-7488D3B97413}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4026,7 +4025,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
@@ -4089,7 +4088,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4112,10 +4111,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4141,16 +4140,16 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5659E6-2685-F344-A125-DB46FCE86ABE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
@@ -4213,7 +4212,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4236,10 +4235,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4265,7 +4264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B14EC0E-8AC4-6540-9E36-1E324072B8AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4336,7 +4335,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4345,10 +4344,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4365,19 +4364,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -4400,7 +4399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4466,7 +4465,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4475,19 +4474,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4504,28 +4503,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4547,7 +4546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4613,7 +4612,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4622,19 +4621,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4651,28 +4650,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4694,7 +4693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4763,7 +4762,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4772,19 +4771,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4801,28 +4800,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4844,7 +4843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -4919,36 +4918,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -4957,7 +4956,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4970,7 +4969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5095,7 +5094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5165,7 +5164,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5174,7 +5173,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -5195,7 +5194,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5204,7 +5203,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -5230,7 +5229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5296,7 +5295,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5305,19 +5304,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5334,7 +5333,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5343,19 +5342,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5377,7 +5376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5386,7 +5385,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5446,7 +5445,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5455,19 +5454,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5484,28 +5483,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5528,7 +5527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5597,22 +5596,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5631,22 +5630,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -5655,7 +5654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5728,22 +5727,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5762,22 +5761,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -5786,7 +5785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5859,19 +5858,19 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5890,19 +5889,19 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5914,7 +5913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -5984,36 +5983,36 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -6022,7 +6021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -6135,10 +6134,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -6162,7 +6161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -6235,7 +6234,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6244,10 +6243,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -6267,7 +6266,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6276,10 +6275,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -6303,21 +6302,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6377,7 +6377,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6386,25 +6386,25 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>26</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6432,28 +6432,28 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>200</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>202</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>204</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
@@ -6474,7 +6474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -6547,7 +6547,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6556,16 +6556,16 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6592,16 +6592,16 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>211</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>62</v>
+        <v>212</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6619,11 +6619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6631,8 +6631,7 @@
     <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6692,7 +6691,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6701,22 +6700,22 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6732,7 +6731,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6741,22 +6740,22 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
added salesforce id to config file
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -674,24 +674,6 @@
     <t>RS_10545 Multi Field WO Search</t>
   </si>
   <si>
-    <t>WO-00005804</t>
-  </si>
-  <si>
-    <t>WO-00005805</t>
-  </si>
-  <si>
-    <t>WO-00005806</t>
-  </si>
-  <si>
-    <t>WO-00005807</t>
-  </si>
-  <si>
-    <t>WO-00005808</t>
-  </si>
-  <si>
-    <t>WO-00005809</t>
-  </si>
-  <si>
     <t>WO-00005810</t>
   </si>
   <si>
@@ -735,6 +717,24 @@
   </si>
   <si>
     <t>WO-00005855</t>
+  </si>
+  <si>
+    <t>WO-00001026</t>
+  </si>
+  <si>
+    <t>WO-00001027</t>
+  </si>
+  <si>
+    <t>WO-00001028</t>
+  </si>
+  <si>
+    <t>WO-00001029</t>
+  </si>
+  <si>
+    <t>WO-00001030</t>
+  </si>
+  <si>
+    <t>WO-00001031</t>
   </si>
 </sst>
 </file>
@@ -1451,10 +1451,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1584,10 +1584,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -6134,7 +6134,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -6306,12 +6306,12 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
@@ -6432,22 +6432,22 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F3" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="J3" t="s">
         <v>37</v>
@@ -6592,16 +6592,16 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6740,22 +6740,22 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="I3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
changes for the Regression
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21206"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_AAA2F84DEB696FDB1BA1BC82E76D20C67CAE66FD" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="28800" windowHeight="16260" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -59,10 +60,15 @@
     <sheet name="RS_2389" sheetId="2" r:id="rId45"/>
     <sheet name="RS_10569" sheetId="15" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -185,6 +191,9 @@
     <t>Work Orders</t>
   </si>
   <si>
+    <t>WO-00005810</t>
+  </si>
+  <si>
     <t>a240t000000GglLAAS</t>
   </si>
   <si>
@@ -227,6 +236,24 @@
     <t>TechName1</t>
   </si>
   <si>
+    <t>WO-00001026</t>
+  </si>
+  <si>
+    <t>WO-00001027</t>
+  </si>
+  <si>
+    <t>WO-00001028</t>
+  </si>
+  <si>
+    <t>WO-00001029</t>
+  </si>
+  <si>
+    <t>WO-00001030</t>
+  </si>
+  <si>
+    <t>WO-00001031</t>
+  </si>
+  <si>
     <t>a240t000000L5IxAAK</t>
   </si>
   <si>
@@ -236,6 +263,18 @@
     <t>WO_SVMX_4</t>
   </si>
   <si>
+    <t>WO-00005834</t>
+  </si>
+  <si>
+    <t>WO-00005835</t>
+  </si>
+  <si>
+    <t>WO-00005836</t>
+  </si>
+  <si>
+    <t>WO-00005837</t>
+  </si>
+  <si>
     <t>RS_10515_Calender_5</t>
   </si>
   <si>
@@ -245,12 +284,42 @@
     <t>WO_SVMX_6</t>
   </si>
   <si>
+    <t>WO-00005850</t>
+  </si>
+  <si>
+    <t>WO-00005851</t>
+  </si>
+  <si>
+    <t>WO-00005852</t>
+  </si>
+  <si>
+    <t>WO-00005853</t>
+  </si>
+  <si>
+    <t>WO-00005854</t>
+  </si>
+  <si>
+    <t>WO-00005855</t>
+  </si>
+  <si>
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
+    <t>WO-00005820</t>
+  </si>
+  <si>
+    <t>WO-00005821</t>
+  </si>
+  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
+    <t>WO-00005826</t>
+  </si>
+  <si>
+    <t>WO-00005827</t>
+  </si>
+  <si>
     <t>SCN_ChecklistOPDOC_3_RS-10587</t>
   </si>
   <si>
@@ -278,9 +347,21 @@
     <t>Default title for Checklist</t>
   </si>
   <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_allversions</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
+  </si>
+  <si>
+    <t>SCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
+  </si>
+  <si>
     <t>AUTO_EDIT_WORKORDER</t>
   </si>
   <si>
+    <t>Auto_SCN_ChecklistOPDOC_3_RS-10587</t>
+  </si>
+  <si>
     <t>SCN_ChecklistOPDOC_1_RS-10585</t>
   </si>
   <si>
@@ -290,6 +371,12 @@
     <t>Data_SCN_ChecklistOPDOC_1_RS-10585</t>
   </si>
   <si>
+    <t>Auto_10585_ChecklistOPDOC</t>
+  </si>
+  <si>
+    <t>Auto_RS10585_ChecklistOPDOC_InProgOP</t>
+  </si>
+  <si>
     <t>SCN_RS_11179</t>
   </si>
   <si>
@@ -305,7 +392,7 @@
     <t>SCN_GetPriceNotCovered_RS_10532</t>
   </si>
   <si>
-    <t>WO-00002804</t>
+    <t>WO-00001032</t>
   </si>
   <si>
     <t>SCN_GetPriceSCON_RS_10539</t>
@@ -326,19 +413,19 @@
     <t>Installed Product Name</t>
   </si>
   <si>
-    <t>WO-00000002</t>
-  </si>
-  <si>
-    <t>P1053915112018111331</t>
-  </si>
-  <si>
-    <t>P1053915112018111332</t>
-  </si>
-  <si>
-    <t>AutoScon1511201811620</t>
-  </si>
-  <si>
-    <t>Auto_10539151120181167</t>
+    <t>WO-00001024</t>
+  </si>
+  <si>
+    <t>P1053910122018953521</t>
+  </si>
+  <si>
+    <t>P1053910122018953522</t>
+  </si>
+  <si>
+    <t>AutoScon1012201810025</t>
+  </si>
+  <si>
+    <t>Auto_105391012201810010</t>
   </si>
   <si>
     <t>IB1053918102018142834</t>
@@ -365,16 +452,16 @@
     <t xml:space="preserve">Product Name </t>
   </si>
   <si>
-    <t>WO-00003464</t>
-  </si>
-  <si>
-    <t>P1053818102018123548</t>
+    <t>WO-00000843</t>
+  </si>
+  <si>
+    <t>P105387122018164340</t>
   </si>
   <si>
     <t>AutoA10538_Auto</t>
   </si>
   <si>
-    <t>IB1053818102018123550</t>
+    <t>IB105387122018164342</t>
   </si>
   <si>
     <t>SCN_ChecklistOPDOC_2_RS-10586</t>
@@ -383,6 +470,12 @@
     <t>Data_SCN_ChecklistOPDOC_2_RS-10586</t>
   </si>
   <si>
+    <t>Auto_10586_ChecklistOPDOC_DynamicRes</t>
+  </si>
+  <si>
+    <t>OPDOC_10586_ChecklistOPDOC_DynamicRes</t>
+  </si>
+  <si>
     <t>RS_10566_Acc_Pro_History</t>
   </si>
   <si>
@@ -437,6 +530,9 @@
     <t>Data_SCN_Checklist_4_RS-10580_Sections</t>
   </si>
   <si>
+    <t>Auto_10580_ChecklistSections</t>
+  </si>
+  <si>
     <t>SCN_ChecklistAttachment_RS-10584</t>
   </si>
   <si>
@@ -452,6 +548,9 @@
     <t>Data_SCN_Checklist_3_RS-10579_Entry_Exit_Criteria</t>
   </si>
   <si>
+    <t>Auto_10579_Checklist</t>
+  </si>
+  <si>
     <t>SCN_Checklist_2_RS-10578_DVR</t>
   </si>
   <si>
@@ -476,6 +575,15 @@
     <t>RS_10554_field_mapping</t>
   </si>
   <si>
+    <t>RS_10549</t>
+  </si>
+  <si>
+    <t>SCN_RS_10549</t>
+  </si>
+  <si>
+    <t>RS_10549 Multi Field WO Search</t>
+  </si>
+  <si>
     <t>RS_10548</t>
   </si>
   <si>
@@ -485,6 +593,15 @@
     <t>RS_10548 Multi Field WO Search</t>
   </si>
   <si>
+    <t>RS_10545</t>
+  </si>
+  <si>
+    <t>SCN_RS_10545</t>
+  </si>
+  <si>
+    <t>RS_10545 Multi Field WO Search</t>
+  </si>
+  <si>
     <t>RS_10543</t>
   </si>
   <si>
@@ -590,6 +707,9 @@
     <t>Cases</t>
   </si>
   <si>
+    <t>Sanity_Scenario6</t>
+  </si>
+  <si>
     <t>SANITY5</t>
   </si>
   <si>
@@ -605,143 +725,29 @@
     <t>Data_Scenario7_Checklist</t>
   </si>
   <si>
+    <t>Sanity7_checklist</t>
+  </si>
+  <si>
+    <t>Checklist_OPDOC</t>
+  </si>
+  <si>
     <t>RS_2389_checklist</t>
   </si>
   <si>
+    <t>Sanity2_Checklist</t>
+  </si>
+  <si>
     <t>SCN_ScheduledDataSync_RS_10569</t>
   </si>
   <si>
     <t>DATA_SCN_ScheduledDataSync_RS_10569</t>
-  </si>
-  <si>
-    <t>Sanity2_Checklist</t>
-  </si>
-  <si>
-    <t>Sanity7_checklist</t>
-  </si>
-  <si>
-    <t>Checklist_OPDOC</t>
-  </si>
-  <si>
-    <t>Sanity_Scenario6</t>
-  </si>
-  <si>
-    <t>RS_10549</t>
-  </si>
-  <si>
-    <t>SCN_RS_10549</t>
-  </si>
-  <si>
-    <t>RS_10549 Multi Field WO Search</t>
-  </si>
-  <si>
-    <t>Auto_10585_ChecklistOPDOC</t>
-  </si>
-  <si>
-    <t>Auto_RS10585_ChecklistOPDOC_InProgOP</t>
-  </si>
-  <si>
-    <t>Auto_10579_Checklist</t>
-  </si>
-  <si>
-    <t>Auto_10580_ChecklistSections</t>
-  </si>
-  <si>
-    <t>Auto_10586_ChecklistOPDOC_DynamicRes</t>
-  </si>
-  <si>
-    <t>OPDOC_10586_ChecklistOPDOC_DynamicRes</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_3_RS-10587_allversions</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_3_RS-10587_firstversion</t>
-  </si>
-  <si>
-    <t>SCN_ChecklistOPDOC_3_RS-10587_lastversion</t>
-  </si>
-  <si>
-    <t>Auto_SCN_ChecklistOPDOC_3_RS-10587</t>
-  </si>
-  <si>
-    <t>RS_10545</t>
-  </si>
-  <si>
-    <t>SCN_RS_10545</t>
-  </si>
-  <si>
-    <t>RS_10545 Multi Field WO Search</t>
-  </si>
-  <si>
-    <t>WO-00005810</t>
-  </si>
-  <si>
-    <t>WO-00005820</t>
-  </si>
-  <si>
-    <t>WO-00005821</t>
-  </si>
-  <si>
-    <t>WO-00005826</t>
-  </si>
-  <si>
-    <t>WO-00005827</t>
-  </si>
-  <si>
-    <t>WO-00005834</t>
-  </si>
-  <si>
-    <t>WO-00005835</t>
-  </si>
-  <si>
-    <t>WO-00005836</t>
-  </si>
-  <si>
-    <t>WO-00005837</t>
-  </si>
-  <si>
-    <t>WO-00005850</t>
-  </si>
-  <si>
-    <t>WO-00005851</t>
-  </si>
-  <si>
-    <t>WO-00005852</t>
-  </si>
-  <si>
-    <t>WO-00005853</t>
-  </si>
-  <si>
-    <t>WO-00005854</t>
-  </si>
-  <si>
-    <t>WO-00005855</t>
-  </si>
-  <si>
-    <t>WO-00001026</t>
-  </si>
-  <si>
-    <t>WO-00001027</t>
-  </si>
-  <si>
-    <t>WO-00001028</t>
-  </si>
-  <si>
-    <t>WO-00001029</t>
-  </si>
-  <si>
-    <t>WO-00001030</t>
-  </si>
-  <si>
-    <t>WO-00001031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,10 +930,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1240,27 +1246,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1321,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1330,7 @@
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1340,20 +1346,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1408,9 +1414,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -1419,10 +1425,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1440,9 +1446,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1451,10 +1457,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>75</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>202</v>
+        <v>76</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1473,20 +1479,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,9 +1547,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -1552,10 +1558,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1573,9 +1579,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1584,10 +1590,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>79</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1606,23 +1612,23 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0" xr3:uid="{FF0BDA26-1AD6-5648-BD9A-E01AA4DDCA7C}">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="42.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1677,62 +1683,62 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>196</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1741,22 +1747,22 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C67EF94B-0B3B-5838-830C-E3A509766221}">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1811,50 +1817,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1863,20 +1869,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{274F5AE0-5452-572F-8038-C13FFDA59D49}">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1884,20 +1890,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1906,16 +1912,20 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0" xr3:uid="{33642244-9AC9-5136-AF77-195C889548CE}">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1970,20 +1980,20 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1992,20 +2002,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D624DF06-3800-545C-AC8D-BADC89115800}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2060,50 +2071,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2112,20 +2123,20 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{11A3ACCB-1F19-5AC9-A611-4158731A345D}">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2133,20 +2144,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="16" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2155,21 +2166,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F1CDC194-CB96-5A2D-8E84-222F42300CFA}">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2180,9 +2191,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2191,15 +2202,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2208,20 +2219,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CF366857-BBDD-5199-9BC9-FF52903B0715}">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2276,38 +2287,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2316,16 +2327,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2391,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2391,7 +2402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2408,21 +2419,21 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{34904945-5288-588E-9F07-34343C13E9F2}">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2477,50 +2488,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>192</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2529,20 +2540,20 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{731C365F-4EDE-5636-9D2D-917179ED8537}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2597,9 +2608,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2608,15 +2619,15 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2625,10 +2636,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2637,16 +2648,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{0801C90D-E949-51CC-9495-7D82D7DEDABF}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2701,30 +2712,30 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2737,19 +2748,19 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{AB5DE215-5931-5800-A1A6-141DC62B4C85}">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2804,38 +2815,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2844,16 +2855,16 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{96AA9D09-0E06-52DD-9EE1-B522AFA11096}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2908,9 +2919,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2919,7 +2930,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>33</v>
@@ -2940,21 +2951,21 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2979,20 +2990,20 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2C1BA805-FFAE-53D9-94C0-3D95D45B0C9C}">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3047,9 +3058,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3058,7 +3069,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3077,18 +3088,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3114,20 +3125,20 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{94BC7849-1D55-59FD-A4A3-F33B65D9F6CB}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3182,44 +3193,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3228,24 +3239,24 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F4A53677-9E12-59C4-BAB1-211CDE2C826E}">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3300,44 +3311,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3346,21 +3357,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{23B2C380-326F-580B-8990-D38B2516F165}">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3415,44 +3426,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3461,21 +3472,21 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{EE242A16-C6B8-5192-B120-522BC795EE76}">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3530,44 +3541,44 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3576,21 +3587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3607,7 +3618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
@@ -3618,7 +3629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3635,22 +3646,22 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{7075697D-051A-5480-9A35-AA80E904E1A1}">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3705,50 +3716,50 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3757,21 +3768,21 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{C7A11F4D-6E51-5B1A-9CF2-8FFD2B06F078}">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3826,9 +3837,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3837,7 +3848,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3856,18 +3867,18 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3892,22 +3903,22 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{D979DC6D-665A-5B40-B235-9A07D260EAB6}">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3962,9 +3973,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3985,12 +3996,12 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4016,22 +4027,22 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{CAA03FB3-9A95-5D50-9E3C-B000AFB1AE50}">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4086,9 +4097,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4109,12 +4120,12 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4140,22 +4151,22 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{62E455AB-44C1-5DAA-A80F-CFF2989D01C0}">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4210,9 +4221,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4233,12 +4244,12 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4264,21 +4275,21 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{E6B2BAC2-667D-5CCD-8069-8C8F7D962337}">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4333,9 +4344,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4344,10 +4355,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -4362,21 +4373,21 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -4399,16 +4410,16 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{BF3E6036-5CFF-541C-9DD1-8B260238869F}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4463,9 +4474,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4474,19 +4485,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4501,30 +4512,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4546,16 +4557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44C9DB06-433C-50F5-8210-7EB2F2901AA3}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4610,9 +4621,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4621,19 +4632,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4648,30 +4659,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4693,19 +4704,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{8CA7FA36-F026-53D8-85D7-7434F22EA588}">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4760,9 +4771,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4771,19 +4782,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4798,30 +4809,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4843,25 +4854,25 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{87752282-9950-53E0-ACC6-858909551C9B}">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4916,38 +4927,38 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -4956,7 +4967,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4969,22 +4980,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5039,7 +5050,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -5067,7 +5078,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -5094,20 +5105,20 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FB84E6B5-2F03-524A-B55D-05F6A9FA1888}">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5162,9 +5173,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5173,7 +5184,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -5192,9 +5203,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5203,7 +5214,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -5229,16 +5240,16 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{FA9D0CF8-F9BB-5117-B023-E36B10EBCA76}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5293,9 +5304,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5304,19 +5315,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5331,9 +5342,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5342,19 +5353,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5376,19 +5387,19 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{62F1EA49-F163-5359-9764-B7CD00A4F86E}">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5443,9 +5454,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -5454,19 +5465,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -5481,30 +5492,30 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5527,19 +5538,19 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{22EC4E50-C5E2-5B45-B3E6-2D2467F4FBB9}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5594,24 +5605,24 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5628,24 +5639,24 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -5654,23 +5665,23 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{701D7CAA-229E-5CB1-96B2-8F6C91020655}">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5725,24 +5736,24 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5759,24 +5770,24 @@
       <c r="S2"/>
       <c r="T2"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -5785,23 +5796,23 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{762215AB-03FA-5155-B868-AA11ECFE6524}">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5856,21 +5867,21 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5887,21 +5898,21 @@
       <c r="R2"/>
       <c r="S2"/>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.95">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5913,23 +5924,23 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{2DFAA6B7-64D6-5785-A35B-5A71D07F531F}">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5981,38 +5992,38 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="8" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -6021,22 +6032,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6091,7 +6102,7 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -6123,7 +6134,7 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -6134,10 +6145,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>200</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -6161,23 +6172,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6232,9 +6243,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6243,10 +6254,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -6264,9 +6275,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6275,10 +6286,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -6302,25 +6313,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6375,9 +6386,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6386,25 +6397,25 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>26</v>
@@ -6421,9 +6432,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6432,28 +6443,28 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>52</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>216</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>219</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
         <v>29</v>
@@ -6474,23 +6485,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6545,9 +6556,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6556,16 +6567,16 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -6581,9 +6592,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6592,16 +6603,16 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>61</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>206</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>207</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>64</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -6619,22 +6630,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6689,9 +6700,9 @@
       <c r="R1"/>
       <c r="S1"/>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -6700,22 +6711,22 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -6729,9 +6740,9 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -6740,22 +6751,22 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>68</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>210</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>213</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>214</v>
+        <v>73</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>

</xml_diff>

<commit_message>
changes for Regression Run
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="232">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -761,12 +761,22 @@
   </si>
   <si>
     <t>OPDOC_10586_ChecklistOPDOC_DynamicRes</t>
+  </si>
+  <si>
+    <t>WO-00005967</t>
+  </si>
+  <si>
+    <t>P1053818122018141912</t>
+  </si>
+  <si>
+    <t>IB1053818122018141914</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1282,15 +1292,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.5" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1382,8 +1392,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1515,8 +1525,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1648,10 +1658,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1760,8 +1770,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1803,7 +1813,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1892,8 +1902,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="30.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2012,8 +2022,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2055,9 +2065,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="50.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2108,8 +2118,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2189,16 +2199,16 @@
         <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
         <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2216,8 +2226,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2516,7 +2526,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2758,8 +2768,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,12 +2903,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3011,9 +3021,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3146,10 +3156,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3270,10 +3280,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3394,9 +3404,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3517,9 +3527,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3652,9 +3662,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -4005,7 +4015,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4155,13 +4165,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4281,8 +4291,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4563,7 +4573,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="27.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4714,7 +4724,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4841,11 +4851,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4949,11 +4959,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5080,10 +5090,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5205,11 +5215,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5333,10 +5343,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5455,9 +5465,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5570,9 +5580,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5685,8 +5695,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5799,11 +5809,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5922,9 +5932,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6043,11 +6053,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="37.1640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="32.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6178,10 +6188,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6318,11 +6328,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6459,12 +6469,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6630,11 +6640,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6775,11 +6785,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added processcheck and commented child SOU as defect wont fix already exists
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B0E9E-109C-624D-91E0-B5E68B8C6740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AF996B-F030-294B-9374-C2D251C0A3D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="33" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="20" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="229">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -430,18 +430,9 @@
     <t xml:space="preserve">Product Name </t>
   </si>
   <si>
-    <t>WO-00003464</t>
-  </si>
-  <si>
-    <t>P1053818102018123548</t>
-  </si>
-  <si>
     <t>AutoA10538_Auto</t>
   </si>
   <si>
-    <t>IB1053818102018123550</t>
-  </si>
-  <si>
     <t>SCN_ChecklistOPDOC_2_RS-10586</t>
   </si>
   <si>
@@ -472,9 +463,6 @@
     <t>Data_SCN_SourceObjectUpdate_RS_10544</t>
   </si>
   <si>
-    <t>Manual_RS_10544_SOU</t>
-  </si>
-  <si>
     <t>RS-10556_mapping</t>
   </si>
   <si>
@@ -770,13 +758,15 @@
   </si>
   <si>
     <t>IB1053818122018141914</t>
+  </si>
+  <si>
+    <t>Auto_RS_10544_SOU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1292,15 +1282,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.1640625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1392,8 +1382,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1525,8 +1515,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1658,10 +1648,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1715,7 +1705,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1727,16 +1717,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -1745,13 +1735,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1770,8 +1760,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1813,7 +1803,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.1640625" collapsed="true"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1902,8 +1892,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="30.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2022,8 +2012,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.5" collapsed="true"/>
+    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2065,9 +2055,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="50.1640625" collapsed="true"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2118,8 +2108,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.83203125" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2199,16 +2189,16 @@
         <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2226,8 +2216,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2287,7 +2277,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2296,7 +2286,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>85</v>
@@ -2304,7 +2294,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2313,10 +2303,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2483,7 +2473,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2498,13 +2488,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2520,13 +2510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.1640625" collapsed="true"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2586,7 +2579,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2603,13 +2596,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>132</v>
+        <v>228</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2690,7 +2683,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2722,19 +2715,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2768,8 +2761,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,7 +2822,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2859,16 +2852,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2903,12 +2896,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2968,7 +2961,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2988,7 +2981,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3000,7 +2993,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -3021,9 +3014,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3083,7 +3076,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3113,16 +3106,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3156,10 +3149,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3219,7 +3212,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3242,10 +3235,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3280,10 +3273,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3343,7 +3336,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3366,10 +3359,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3404,9 +3397,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3466,7 +3459,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3489,10 +3482,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3527,9 +3520,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3589,7 +3582,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3601,7 +3594,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -3618,19 +3611,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3662,9 +3655,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3778,7 +3771,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3790,16 +3783,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3816,28 +3809,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3925,7 +3918,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3937,16 +3930,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3963,28 +3956,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4015,7 +4008,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4075,7 +4068,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4087,16 +4080,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4113,28 +4106,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4165,13 +4158,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4231,7 +4224,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4243,18 +4236,18 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4269,7 +4262,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4291,8 +4284,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.83203125" collapsed="true"/>
+    <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4352,7 +4345,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4382,7 +4375,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4391,7 +4384,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4483,7 +4476,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4495,16 +4488,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4521,7 +4514,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4530,19 +4523,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4573,7 +4566,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="4" max="4" width="27.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4633,7 +4626,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4645,16 +4638,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4671,28 +4664,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4724,7 +4717,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4784,7 +4777,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4796,10 +4789,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4818,22 +4811,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4851,11 +4844,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="42.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4912,7 +4905,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4929,7 +4922,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4959,11 +4952,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5023,7 +5016,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5057,7 +5050,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5069,10 +5062,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -5090,10 +5083,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5215,11 +5208,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5279,7 +5272,7 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5310,7 +5303,7 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5322,7 +5315,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5343,10 +5336,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5406,7 +5399,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5429,7 +5422,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5441,10 +5434,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>89</v>
@@ -5465,9 +5458,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5527,7 +5520,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5547,7 +5540,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5559,7 +5552,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5580,9 +5573,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5642,7 +5635,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5662,7 +5655,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5674,7 +5667,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5695,8 +5688,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5756,7 +5749,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5776,7 +5769,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5788,7 +5781,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5809,11 +5802,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5908,13 +5901,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -5926,15 +5919,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5994,7 +5987,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -6017,7 +6010,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -6029,13 +6022,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -6053,11 +6046,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="37.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="37.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6158,19 +6151,19 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6188,10 +6181,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6328,11 +6321,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6469,12 +6462,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6640,11 +6633,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6785,11 +6778,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updating changes to checklist
This reverts commit a3ba0eac41693b66709ba8e72b11ae00816cfaa4.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/SVMX_Catalyst/fsaautomation/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AF996B-F030-294B-9374-C2D251C0A3D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E937B4-5B4E-E448-B228-6B9F8CBCEB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="20" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="30" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="229">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -391,21 +391,6 @@
     <t>Installed Product Name</t>
   </si>
   <si>
-    <t>WO-00000002</t>
-  </si>
-  <si>
-    <t>P1053915112018111331</t>
-  </si>
-  <si>
-    <t>P1053915112018111332</t>
-  </si>
-  <si>
-    <t>AutoScon1511201811620</t>
-  </si>
-  <si>
-    <t>Auto_10539151120181167</t>
-  </si>
-  <si>
     <t>IB1053918102018142834</t>
   </si>
   <si>
@@ -697,9 +682,6 @@
     <t>Auto_10579_Checklist</t>
   </si>
   <si>
-    <t>Auto_10580_ChecklistSections</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -751,15 +733,6 @@
     <t>OPDOC_10586_ChecklistOPDOC_DynamicRes</t>
   </si>
   <si>
-    <t>WO-00005967</t>
-  </si>
-  <si>
-    <t>P1053818122018141912</t>
-  </si>
-  <si>
-    <t>IB1053818122018141914</t>
-  </si>
-  <si>
     <t>Auto_RS_10544_SOU</t>
   </si>
   <si>
@@ -785,13 +758,15 @@
   </si>
   <si>
     <t>Auto_1053928122018122610</t>
+  </si>
+  <si>
+    <t>Automation_10580_ChecklistSections</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1307,15 +1282,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.1640625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1407,8 +1382,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,8 +1515,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1673,10 +1648,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1730,7 +1705,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -1742,16 +1717,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -1760,13 +1735,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1785,8 +1760,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1828,7 +1803,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.1640625" collapsed="true"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,8 +1892,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="30.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="6" max="6" width="30.5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2004,22 +1979,22 @@
         <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2037,8 +2012,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.5" collapsed="true"/>
+    <col min="1" max="1" width="29.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2051,7 +2026,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2059,10 +2034,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2080,9 +2055,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="50.1640625" collapsed="true"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,7 +2073,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2109,13 +2084,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2133,8 +2108,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.83203125" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2194,13 +2169,13 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>103</v>
@@ -2211,19 +2186,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2241,8 +2216,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2302,7 +2277,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2311,7 +2286,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>85</v>
@@ -2319,7 +2294,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2328,10 +2303,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2498,7 +2473,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2513,13 +2488,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2535,16 +2510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2604,7 +2579,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -2621,13 +2596,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
@@ -2708,7 +2683,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2740,19 +2715,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2786,8 +2761,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2847,7 +2822,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -2877,16 +2852,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2921,12 +2896,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2986,7 +2961,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -3006,7 +2981,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -3018,7 +2993,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -3039,9 +3014,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.1640625" collapsed="true"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3101,7 +3076,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3131,16 +3106,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3174,10 +3149,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3237,7 +3212,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3260,10 +3235,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3298,10 +3273,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3361,7 +3336,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3384,10 +3359,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3422,9 +3397,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3484,7 +3459,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3507,10 +3482,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3545,9 +3520,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="49.1640625" collapsed="true"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3607,7 +3582,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3619,7 +3594,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -3636,19 +3611,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3680,9 +3655,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3796,7 +3771,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3808,16 +3783,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3834,28 +3809,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3943,7 +3918,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -3955,16 +3930,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3981,28 +3956,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4033,7 +4008,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4093,7 +4068,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4105,16 +4080,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4131,28 +4106,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4183,13 +4158,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4249,7 +4224,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4261,18 +4236,18 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4287,7 +4262,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4309,8 +4284,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.83203125" collapsed="true"/>
+    <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4370,7 +4345,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4400,7 +4375,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4409,7 +4384,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4501,7 +4476,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4513,16 +4488,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4539,7 +4514,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4548,19 +4523,19 @@
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4591,7 +4566,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="4" max="4" width="27.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4651,7 +4626,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>31</v>
@@ -4663,16 +4638,16 @@
         <v>81</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4689,28 +4664,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4742,7 +4717,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4802,7 +4777,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4814,10 +4789,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4836,22 +4811,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4869,11 +4844,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="42.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4930,7 +4905,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -4947,7 +4922,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -4977,11 +4952,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5041,7 +5016,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5075,7 +5050,7 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5087,10 +5062,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5108,10 +5083,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5233,11 +5208,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5297,7 +5272,7 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5328,7 +5303,7 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5340,7 +5315,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5361,10 +5336,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="32.1640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5424,7 +5399,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5447,7 +5422,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5459,10 +5434,10 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>89</v>
@@ -5483,9 +5458,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5545,7 +5520,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5565,7 +5540,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5577,7 +5552,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5598,9 +5573,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5660,7 +5635,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5680,7 +5655,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5692,7 +5667,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5707,14 +5682,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5774,7 +5749,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -5794,7 +5769,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -5806,7 +5781,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
@@ -5827,11 +5802,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5926,13 +5901,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5950,9 +5925,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6012,7 +5987,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -6035,7 +6010,7 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -6047,13 +6022,13 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -6071,11 +6046,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="37.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="37.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6176,19 +6151,19 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -6206,10 +6181,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6346,11 +6321,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6487,12 +6462,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6658,11 +6633,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6803,11 +6778,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/yadavsvmx/SVMX_Catalyst"
This reverts commit 2414d7d7ee4cbf586e713520cd2b89365b29b538, reversing
changes made to 39662fe4d26c625de13d627eafd0726b4741a996.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="9" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="235">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -294,12 +294,6 @@
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
-    <t>WO-00004367</t>
-  </si>
-  <si>
-    <t>WO-00004368</t>
-  </si>
-  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
@@ -768,34 +762,22 @@
     <t>0053D000001fEk6QAE</t>
   </si>
   <si>
-    <t>WO-00012789</t>
-  </si>
-  <si>
-    <t>WO-00012790</t>
-  </si>
-  <si>
-    <t>WO-00012791</t>
-  </si>
-  <si>
-    <t>WO-00012792</t>
-  </si>
-  <si>
-    <t>WO-00012832</t>
-  </si>
-  <si>
-    <t>WO-00012833</t>
-  </si>
-  <si>
-    <t>WO-00012840</t>
-  </si>
-  <si>
-    <t>WO-00012841</t>
-  </si>
-  <si>
     <t>WO-00012845</t>
   </si>
   <si>
     <t>WO-00012846</t>
+  </si>
+  <si>
+    <t>WO-00013370</t>
+  </si>
+  <si>
+    <t>WO-00013371</t>
+  </si>
+  <si>
+    <t>WO-00013372</t>
+  </si>
+  <si>
+    <t>WO-00013373</t>
   </si>
 </sst>
 </file>
@@ -1527,10 +1509,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1619,7 +1601,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -1651,7 +1633,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -1660,10 +1642,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1748,7 +1730,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
@@ -1757,19 +1739,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -1778,13 +1760,13 @@
         <v>34</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>202</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1817,18 +1799,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1906,7 +1888,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1914,10 +1896,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1996,48 +1978,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" t="s">
         <v>221</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>222</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>223</v>
       </c>
-      <c r="E3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" t="s">
-        <v>225</v>
-      </c>
       <c r="G3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2069,7 +2051,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2077,10 +2059,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2116,7 +2098,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2127,13 +2109,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
         <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2212,36 +2194,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>218</v>
-      </c>
-      <c r="C3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2320,7 +2302,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2329,15 +2311,15 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -2346,10 +2328,10 @@
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2516,13 +2498,13 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
@@ -2531,13 +2513,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
@@ -2622,36 +2604,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2726,7 +2708,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2735,7 +2717,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>31</v>
@@ -2758,19 +2740,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
         <v>121</v>
-      </c>
-      <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>123</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2865,7 +2847,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2874,7 +2856,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2895,16 +2877,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -3004,42 +2986,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3051,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3119,7 +3101,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3128,7 +3110,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3149,16 +3131,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3255,7 +3237,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3278,10 +3260,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3379,7 +3361,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3402,10 +3384,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3502,7 +3484,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3525,10 +3507,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3625,7 +3607,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3634,10 +3616,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -3654,19 +3636,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3736,10 +3718,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3814,7 +3796,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3823,19 +3805,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3852,28 +3834,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3961,7 +3943,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3970,19 +3952,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3999,28 +3981,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4111,7 +4093,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4120,19 +4102,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4149,28 +4131,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4267,36 +4249,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
@@ -4305,7 +4287,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4388,7 +4370,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4397,7 +4379,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -4418,7 +4400,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -4427,7 +4409,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4519,7 +4501,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4528,19 +4510,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4557,7 +4539,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -4566,19 +4548,19 @@
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4669,7 +4651,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4678,19 +4660,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4707,28 +4689,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4820,22 +4802,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4854,22 +4836,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4948,36 +4930,36 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5059,22 +5041,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5093,22 +5075,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -5120,7 +5102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5223,7 +5205,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E3" s="17"/>
       <c r="M3" s="8"/>
@@ -5315,19 +5297,19 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5346,19 +5328,19 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5442,48 +5424,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5563,42 +5545,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5678,42 +5660,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5792,42 +5774,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5909,48 +5891,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -6030,48 +6012,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -6153,60 +6135,60 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" t="s">
         <v>209</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" t="s">
         <v>210</v>
-      </c>
-      <c r="G3" t="s">
-        <v>211</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/yadavsvmx/SVMX_Catalyst""
This reverts commit e30cef90cdb4037035410e6d7dd21933cb3ca5b1.
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="9" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16260" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RS_10537" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="241">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -294,6 +294,12 @@
     <t>RS_10513_Calender_3</t>
   </si>
   <si>
+    <t>WO-00004367</t>
+  </si>
+  <si>
+    <t>WO-00004368</t>
+  </si>
+  <si>
     <t>RS_11859_Calender_3</t>
   </si>
   <si>
@@ -762,22 +768,34 @@
     <t>0053D000001fEk6QAE</t>
   </si>
   <si>
+    <t>WO-00012789</t>
+  </si>
+  <si>
+    <t>WO-00012790</t>
+  </si>
+  <si>
+    <t>WO-00012791</t>
+  </si>
+  <si>
+    <t>WO-00012792</t>
+  </si>
+  <si>
+    <t>WO-00012832</t>
+  </si>
+  <si>
+    <t>WO-00012833</t>
+  </si>
+  <si>
+    <t>WO-00012840</t>
+  </si>
+  <si>
+    <t>WO-00012841</t>
+  </si>
+  <si>
     <t>WO-00012845</t>
   </si>
   <si>
     <t>WO-00012846</t>
-  </si>
-  <si>
-    <t>WO-00013370</t>
-  </si>
-  <si>
-    <t>WO-00013371</t>
-  </si>
-  <si>
-    <t>WO-00013372</t>
-  </si>
-  <si>
-    <t>WO-00013373</t>
   </si>
 </sst>
 </file>
@@ -1509,10 +1527,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1601,7 +1619,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -1633,7 +1651,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -1642,10 +1660,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1730,7 +1748,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
@@ -1739,19 +1757,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -1760,13 +1778,13 @@
         <v>34</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1799,18 +1817,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1906,7 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
@@ -1896,10 +1914,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1978,48 +1996,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2069,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2059,10 +2077,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2098,7 +2116,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
@@ -2109,13 +2127,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2194,36 +2212,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2302,7 +2320,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2311,15 +2329,15 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -2328,10 +2346,10 @@
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2498,13 +2516,13 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
@@ -2513,13 +2531,13 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
@@ -2604,36 +2622,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2708,7 +2726,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2717,7 +2735,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>31</v>
@@ -2740,19 +2758,19 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2847,7 +2865,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -2856,7 +2874,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2877,16 +2895,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2986,42 +3004,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3033,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3101,7 +3119,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3110,7 +3128,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3131,16 +3149,16 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3237,7 +3255,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3260,10 +3278,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3361,7 +3379,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3384,10 +3402,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3484,7 +3502,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3507,10 +3525,10 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3607,7 +3625,7 @@
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3616,10 +3634,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -3636,19 +3654,19 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3718,10 +3736,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3796,7 +3814,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3805,19 +3823,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3834,28 +3852,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3943,7 +3961,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -3952,19 +3970,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3981,28 +3999,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4093,7 +4111,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4102,19 +4120,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4131,28 +4149,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4249,36 +4267,36 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
@@ -4287,7 +4305,7 @@
         <v>43466</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G3" s="8">
         <v>10</v>
@@ -4370,7 +4388,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4379,7 +4397,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -4400,7 +4418,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -4409,7 +4427,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -4501,7 +4519,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4510,19 +4528,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4539,7 +4557,7 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
@@ -4548,19 +4566,19 @@
         <v>34</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4651,7 +4669,7 @@
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>29</v>
@@ -4660,19 +4678,19 @@
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -4689,28 +4707,28 @@
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -4802,22 +4820,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4836,22 +4854,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4930,36 +4948,36 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5041,22 +5059,22 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5075,22 +5093,22 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -5102,7 +5120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5205,7 +5223,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E3" s="17"/>
       <c r="M3" s="8"/>
@@ -5297,19 +5315,19 @@
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -5328,19 +5346,19 @@
     </row>
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="6"/>
@@ -5424,48 +5442,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5545,42 +5563,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5660,42 +5678,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5774,42 +5792,42 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -5891,48 +5909,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -6012,48 +6030,48 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -6135,60 +6153,60 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add salesforce id to config file
</commit_message>
<xml_diff>
--- a/fsaautomation/resources/TestData.xlsx
+++ b/fsaautomation/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212718562\Documents\Newpull\"/>
     </mc:Choice>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="237">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -781,12 +781,19 @@
   </si>
   <si>
     <t>Data_SCN_Workoreder_Attachment_RS-9726</t>
+  </si>
+  <si>
+    <t>WO-00016047</t>
+  </si>
+  <si>
+    <t>WO-00016048</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -1309,15 +1316,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1409,8 +1416,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1542,8 +1549,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1644,10 +1651,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>235</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>236</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1675,10 +1682,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1787,8 +1794,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1830,7 +1837,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -1919,8 +1926,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="30.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" customWidth="true" width="30.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2039,8 +2046,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2082,9 +2089,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="50.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2135,8 +2142,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2243,8 +2250,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2543,10 +2550,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2788,8 +2795,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -2923,12 +2930,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3041,9 +3048,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3176,10 +3183,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3300,10 +3307,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3424,9 +3431,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3547,9 +3554,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="46.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="49.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -3682,9 +3689,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4035,7 +4042,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4185,13 +4192,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4311,8 +4318,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4593,7 +4600,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="27.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4744,7 +4751,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4871,11 +4878,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4979,11 +4986,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5110,10 +5117,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5235,11 +5242,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5363,10 +5370,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5485,9 +5492,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5600,9 +5607,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="40.77734375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5715,8 +5722,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5829,11 +5836,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -5952,9 +5959,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="36.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -6073,11 +6080,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="32.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
@@ -6208,12 +6215,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -6328,13 +6335,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="54.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="54.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6417,10 +6424,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -6557,11 +6564,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -6698,12 +6705,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -6869,11 +6876,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">
@@ -7014,11 +7021,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1">

</xml_diff>